<commit_message>
Add HBVCALIB=46 for the Clear Lake drainage at the head of the McKenzie. Flow.xml - Comment out the reference to Flow_WRB_31yr_spinup_2010.ic. Need to do a new spinup using current flow code. HBV.csv - Add parameter values for HBVCALIB 46, copied from those for HBVCALIB 9, the Blue R. Reservoir drainage. IDU.xml - Add an entry for HBVCALIB 46. IDU_McKenzie.dbf and Reach_McKenzie.dbf - Populate HBVCALIB 46 locations. Reach_CW3M.dbf - Populate HBVCALIB 46 locations. This was also done for IDU_CW3M.dbf, which is too big for the GitHub repository. EnvLoader.cpp - Refine an error message. WaterRights.cpp - Add HBVCALIB 46 for the Clear Lake drainage, with the pour point at 23773373. Add and then comment out a call to PopulateHBVCALIB().
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4671E16-3185-49BD-ADA2-1E45FD75958C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55B4787-A448-4318-B85E-2310DFAECDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="765" windowWidth="18405" windowHeight="13050" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature values" sheetId="1" r:id="rId1"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
   <si>
     <t>HBV parameter ranges</t>
   </si>
@@ -441,6 +441,12 @@
   </si>
   <si>
     <t>from 29 Willamette above Salem</t>
+  </si>
+  <si>
+    <t>Clear Lake drainage on McKenzie</t>
+  </si>
+  <si>
+    <t>from 9 Blue River Reservoir drainage</t>
   </si>
 </sst>
 </file>
@@ -1527,30 +1533,30 @@
       <selection pane="bottomRight" activeCell="A29" sqref="A29:XFD31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="3" width="7.5703125" style="9" customWidth="1"/>
-    <col min="4" max="5" width="9.140625" style="24"/>
-    <col min="6" max="7" width="9.140625" style="25"/>
-    <col min="8" max="9" width="9.140625" style="9"/>
-    <col min="10" max="11" width="9.140625" style="30"/>
-    <col min="12" max="13" width="9.140625" style="21"/>
-    <col min="14" max="19" width="9.140625" style="24"/>
-    <col min="20" max="20" width="18.28515625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.109375" customWidth="1"/>
+    <col min="2" max="3" width="7.5546875" style="9" customWidth="1"/>
+    <col min="4" max="5" width="9.109375" style="24"/>
+    <col min="6" max="7" width="9.109375" style="25"/>
+    <col min="8" max="9" width="9.109375" style="9"/>
+    <col min="10" max="11" width="9.109375" style="30"/>
+    <col min="12" max="13" width="9.109375" style="21"/>
+    <col min="14" max="19" width="9.109375" style="24"/>
+    <col min="20" max="20" width="18.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
@@ -1607,7 +1613,7 @@
       </c>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="17" t="s">
         <v>2</v>
       </c>
@@ -1667,7 +1673,7 @@
       </c>
       <c r="U5" s="5"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1729,7 +1735,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1773,7 +1779,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
@@ -1937,7 +1943,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="23"/>
@@ -1958,7 +1964,7 @@
       <c r="S11" s="23"/>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -2018,7 +2024,7 @@
       </c>
       <c r="T12" s="6"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2047,7 +2053,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2085,7 +2091,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2123,12 +2129,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B16" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2160,7 +2166,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2192,7 +2198,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2224,7 +2230,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2256,7 +2262,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2288,7 +2294,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2320,7 +2326,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2352,7 +2358,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -2384,7 +2390,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2416,12 +2422,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="K26" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2509,28 +2515,28 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N51"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:L24"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C45" sqref="C45:L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.28515625" customWidth="1"/>
-    <col min="2" max="2" width="5.7109375" customWidth="1"/>
-    <col min="3" max="3" width="7.5703125" style="24" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.140625" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6.7109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" style="24"/>
-    <col min="13" max="13" width="12.7109375" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="5.6640625" customWidth="1"/>
+    <col min="3" max="3" width="7.5546875" style="24" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="6.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" style="24"/>
+    <col min="13" max="13" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B1" s="51" t="s">
         <v>45</v>
       </c>
@@ -2565,7 +2571,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="50"/>
       <c r="C2" s="52" t="s">
         <v>17</v>
@@ -2601,7 +2607,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>81</v>
       </c>
@@ -2640,7 +2646,7 @@
       </c>
       <c r="M3" s="5"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>59</v>
       </c>
@@ -2678,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>60</v>
       </c>
@@ -2716,7 +2722,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>61</v>
       </c>
@@ -2754,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>62</v>
       </c>
@@ -2792,7 +2798,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>63</v>
       </c>
@@ -2830,7 +2836,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>64</v>
       </c>
@@ -2868,7 +2874,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>65</v>
       </c>
@@ -2906,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>66</v>
       </c>
@@ -2944,7 +2950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>67</v>
       </c>
@@ -2982,7 +2988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>79</v>
       </c>
@@ -3020,7 +3026,7 @@
         <v>1.3233600000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="67" t="s">
         <v>88</v>
       </c>
@@ -3075,7 +3081,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="67" t="s">
         <v>87</v>
       </c>
@@ -3130,7 +3136,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="67" t="s">
         <v>89</v>
       </c>
@@ -3185,7 +3191,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="67" t="s">
         <v>90</v>
       </c>
@@ -3240,7 +3246,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="58" t="s">
         <v>91</v>
       </c>
@@ -3295,7 +3301,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="58" t="s">
         <v>92</v>
       </c>
@@ -3350,7 +3356,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="75" t="s">
         <v>93</v>
       </c>
@@ -3405,7 +3411,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="58" t="s">
         <v>94</v>
       </c>
@@ -3413,7 +3419,7 @@
         <v>22</v>
       </c>
       <c r="C21" s="60">
-        <f t="shared" ref="C20:C21" si="5">C$3</f>
+        <f t="shared" ref="C21" si="5">C$3</f>
         <v>6</v>
       </c>
       <c r="D21" s="61">
@@ -3460,7 +3466,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>86</v>
       </c>
@@ -3501,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="58" t="s">
         <v>95</v>
       </c>
@@ -3556,7 +3562,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="58" t="s">
         <v>96</v>
       </c>
@@ -3604,14 +3610,14 @@
         <v>1</v>
       </c>
       <c r="M24" s="64">
-        <f t="shared" ref="D24:M24" si="7">M$34</f>
+        <f t="shared" ref="M24" si="7">M$34</f>
         <v>0</v>
       </c>
       <c r="N24" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="58" t="s">
         <v>97</v>
       </c>
@@ -3666,7 +3672,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>78</v>
       </c>
@@ -3704,7 +3710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>68</v>
       </c>
@@ -3742,7 +3748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
       <c r="B28" s="5">
         <v>29</v>
       </c>
@@ -3777,7 +3783,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>77</v>
       </c>
@@ -3815,7 +3821,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>102</v>
       </c>
@@ -3870,7 +3876,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="58" t="s">
         <v>98</v>
       </c>
@@ -3925,7 +3931,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>103</v>
       </c>
@@ -3980,7 +3986,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>85</v>
       </c>
@@ -4021,7 +4027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>69</v>
       </c>
@@ -4059,7 +4065,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>70</v>
       </c>
@@ -4097,7 +4103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>71</v>
       </c>
@@ -4135,7 +4141,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
         <v>72</v>
       </c>
@@ -4173,7 +4179,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
         <v>73</v>
       </c>
@@ -4211,7 +4217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>74</v>
       </c>
@@ -4249,7 +4255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>75</v>
       </c>
@@ -4287,7 +4293,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>76</v>
       </c>
@@ -4325,7 +4331,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>82</v>
       </c>
@@ -4363,7 +4369,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>80</v>
       </c>
@@ -4401,7 +4407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>83</v>
       </c>
@@ -4439,209 +4445,250 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A45" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B45" s="5">
+        <v>46</v>
+      </c>
+      <c r="C45" s="60">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="D45" s="61">
+        <v>5.4128975000000003E-2</v>
+      </c>
+      <c r="E45" s="62">
+        <v>219.77199999999999</v>
+      </c>
+      <c r="F45" s="60">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="G45" s="60">
+        <v>0.188</v>
+      </c>
+      <c r="H45" s="60">
+        <v>4.4269999999999996</v>
+      </c>
+      <c r="I45" s="63">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="J45" s="63">
+        <v>0.26</v>
+      </c>
+      <c r="K45" s="63">
+        <v>0.03</v>
+      </c>
+      <c r="L45" s="60">
+        <v>1</v>
+      </c>
+      <c r="N45" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>56</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="24">
+      <c r="B47" s="9"/>
+      <c r="C47" s="24">
         <v>2.3140000000000001</v>
-      </c>
-      <c r="D46" s="36">
-        <v>0.05</v>
-      </c>
-      <c r="E46" s="21">
-        <v>85</v>
-      </c>
-      <c r="F46" s="24">
-        <v>2.15</v>
-      </c>
-      <c r="G46" s="24">
-        <v>9.4000000000000004E-3</v>
-      </c>
-      <c r="H46" s="9">
-        <v>7.9</v>
-      </c>
-      <c r="I46" s="30">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="J46" s="30">
-        <v>0.03</v>
-      </c>
-      <c r="K46" s="30">
-        <v>2E-3</v>
-      </c>
-      <c r="M46" s="9"/>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>57</v>
-      </c>
-      <c r="C47" s="24">
-        <v>3.72776</v>
       </c>
       <c r="D47" s="36">
         <v>0.05</v>
       </c>
       <c r="E47" s="21">
+        <v>85</v>
+      </c>
+      <c r="F47" s="24">
+        <v>2.15</v>
+      </c>
+      <c r="G47" s="24">
+        <v>9.4000000000000004E-3</v>
+      </c>
+      <c r="H47" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="I47" s="30">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="J47" s="30">
+        <v>0.03</v>
+      </c>
+      <c r="K47" s="30">
+        <v>2E-3</v>
+      </c>
+      <c r="M47" s="9"/>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="24">
+        <v>3.72776</v>
+      </c>
+      <c r="D48" s="36">
+        <v>0.05</v>
+      </c>
+      <c r="E48" s="21">
         <v>456</v>
       </c>
-      <c r="F47" s="24">
+      <c r="F48" s="24">
         <v>4.24</v>
       </c>
-      <c r="G47" s="24">
+      <c r="G48" s="24">
         <v>0.03</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H48" s="9">
         <v>86.6</v>
       </c>
-      <c r="I47" s="30">
+      <c r="I48" s="30">
         <v>0.48</v>
       </c>
-      <c r="J47" s="30">
+      <c r="J48" s="30">
         <v>0.317</v>
       </c>
-      <c r="K47" s="30">
+      <c r="K48" s="30">
         <v>0.105</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="C48" s="24">
+      <c r="C49" s="24">
         <v>4.5944700000000003</v>
       </c>
-      <c r="D48" s="36">
+      <c r="D49" s="36">
         <v>8.4928500000000004E-2</v>
       </c>
-      <c r="E48" s="21">
+      <c r="E49" s="21">
         <v>403.43</v>
       </c>
-      <c r="F48" s="24">
+      <c r="F49" s="24">
         <v>3.6036649999999999</v>
       </c>
-      <c r="G48" s="24">
+      <c r="G49" s="24">
         <v>1.5616099999999999</v>
       </c>
-      <c r="H48" s="9">
+      <c r="H49" s="9">
         <v>45.967799999999997</v>
       </c>
-      <c r="I48" s="30">
+      <c r="I49" s="30">
         <v>0.51648300000000003</v>
       </c>
-      <c r="J48" s="30">
+      <c r="J49" s="30">
         <v>0.13280749999999999</v>
       </c>
-      <c r="K48" s="30">
+      <c r="K49" s="30">
         <v>6.1253000000000002E-2</v>
       </c>
-      <c r="M48" s="5" t="s">
+      <c r="M49" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C50" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="D49" s="36">
+      <c r="D50" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="E49" s="21">
+      <c r="E50" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="F49" s="24">
+      <c r="F50" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="G49" s="24">
+      <c r="G50" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H50" s="9">
         <v>48.445349999999998</v>
       </c>
-      <c r="I49" s="30">
+      <c r="I50" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="J49" s="30">
+      <c r="J50" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="K49" s="30">
+      <c r="K50" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="M49" s="5" t="s">
+      <c r="M50" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>50</v>
-      </c>
-      <c r="C50" s="24">
-        <v>2.5</v>
-      </c>
-      <c r="D50" s="36">
-        <v>5.3031000000000002E-2</v>
-      </c>
-      <c r="E50" s="21">
-        <v>302.19299999999998</v>
-      </c>
-      <c r="F50" s="24">
-        <v>3.3146300000000002</v>
-      </c>
-      <c r="G50" s="24">
-        <v>0.40926699999999999</v>
-      </c>
-      <c r="H50" s="9">
-        <v>6.09443</v>
-      </c>
-      <c r="I50" s="30">
-        <v>0.24992800000000001</v>
-      </c>
-      <c r="J50" s="30">
-        <v>0.24191099999999999</v>
-      </c>
-      <c r="K50" s="30">
-        <v>8.1710000000000005E-2</v>
-      </c>
-      <c r="M50" s="5" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>51</v>
       </c>
       <c r="C51" s="24">
         <v>2.5</v>
       </c>
       <c r="D51" s="36">
+        <v>5.3031000000000002E-2</v>
+      </c>
+      <c r="E51" s="21">
+        <v>302.19299999999998</v>
+      </c>
+      <c r="F51" s="24">
+        <v>3.3146300000000002</v>
+      </c>
+      <c r="G51" s="24">
+        <v>0.40926699999999999</v>
+      </c>
+      <c r="H51" s="9">
+        <v>6.09443</v>
+      </c>
+      <c r="I51" s="30">
+        <v>0.24992800000000001</v>
+      </c>
+      <c r="J51" s="30">
+        <v>0.24191099999999999</v>
+      </c>
+      <c r="K51" s="30">
+        <v>8.1710000000000005E-2</v>
+      </c>
+      <c r="M51" s="5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="24">
+        <v>2.5</v>
+      </c>
+      <c r="D52" s="36">
         <v>2.8663500000000001E-2</v>
       </c>
-      <c r="E51" s="21">
+      <c r="E52" s="21">
         <v>51.938099999999999</v>
       </c>
-      <c r="F51" s="24">
+      <c r="F52" s="24">
         <v>2.2341899999999999</v>
       </c>
-      <c r="G51" s="24">
+      <c r="G52" s="24">
         <v>3.267137</v>
       </c>
-      <c r="H51" s="9">
+      <c r="H52" s="9">
         <v>46.490699999999997</v>
       </c>
-      <c r="I51" s="30">
+      <c r="I52" s="30">
         <v>0.25806499999999999</v>
       </c>
-      <c r="J51" s="30">
+      <c r="J52" s="30">
         <v>7.5115000000000001E-2</v>
       </c>
-      <c r="K51" s="30">
+      <c r="K52" s="30">
         <v>4.5275999999999997E-2</v>
       </c>
-      <c r="M51" s="5" t="s">
+      <c r="M52" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4653,19 +4700,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0CD360-4B2D-45D8-A256-EB9315888EC1}">
-  <dimension ref="A1:L47"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="F48" sqref="F48:G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="9.140625" style="24"/>
-    <col min="6" max="7" width="9.140625" style="36"/>
+    <col min="5" max="5" width="9.109375" style="24"/>
+    <col min="6" max="7" width="9.109375" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="51" t="s">
         <v>45</v>
       </c>
@@ -4703,7 +4750,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -4741,7 +4788,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -4779,7 +4826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -4817,7 +4864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -4855,7 +4902,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -4893,7 +4940,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -4931,7 +4978,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -4969,7 +5016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -5007,7 +5054,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -5045,7 +5092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -5083,7 +5130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -5121,7 +5168,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -5159,7 +5206,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -5197,7 +5244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="50">
         <v>13</v>
       </c>
@@ -5235,7 +5282,7 @@
         <v>1.3233600000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -5273,7 +5320,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -5321,7 +5368,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" s="59">
         <v>16</v>
       </c>
@@ -5369,7 +5416,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="59">
         <v>17</v>
       </c>
@@ -5417,7 +5464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="59">
         <v>18</v>
       </c>
@@ -5465,7 +5512,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="59">
         <v>19</v>
       </c>
@@ -5513,7 +5560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="59">
         <v>20</v>
       </c>
@@ -5561,7 +5608,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="59">
         <v>21</v>
       </c>
@@ -5609,7 +5656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" s="59">
         <v>22</v>
       </c>
@@ -5657,7 +5704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" s="50">
         <v>23</v>
       </c>
@@ -5695,7 +5742,7 @@
         <v>1.93418479</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" s="59">
         <v>24</v>
       </c>
@@ -5743,7 +5790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="59">
         <v>25</v>
       </c>
@@ -5791,7 +5838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="59">
         <v>26</v>
       </c>
@@ -5839,7 +5886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -5877,7 +5924,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -5915,7 +5962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -5953,7 +6000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -5991,7 +6038,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -6039,7 +6086,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -6087,7 +6134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -6125,7 +6172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -6163,7 +6210,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -6201,7 +6248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -6239,7 +6286,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -6277,7 +6324,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -6315,7 +6362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -6353,7 +6400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -6391,7 +6438,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -6429,7 +6476,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -6467,7 +6514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -6505,7 +6552,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -6543,7 +6590,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -6578,6 +6625,44 @@
         <v>5.9999999999999995E-4</v>
       </c>
       <c r="L47" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="5">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3">
+        <v>0</v>
+      </c>
+      <c r="C48" s="60">
+        <v>2.5299999999999998</v>
+      </c>
+      <c r="D48" s="61">
+        <v>5.4128975000000003E-2</v>
+      </c>
+      <c r="E48" s="60">
+        <v>219.77199999999999</v>
+      </c>
+      <c r="F48" s="61">
+        <v>1.1459999999999999</v>
+      </c>
+      <c r="G48" s="61">
+        <v>0.188</v>
+      </c>
+      <c r="H48" s="60">
+        <v>4.4269999999999996</v>
+      </c>
+      <c r="I48" s="63">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="J48" s="63">
+        <v>0.26</v>
+      </c>
+      <c r="K48" s="63">
+        <v>0.03</v>
+      </c>
+      <c r="L48" s="60">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add 3 HBVCALIBs: Smith47, SFork48, and Lookout49. Move the pour point for Mohawk25 from 23773507, Mohawk's outlet into the McKenzie, to 23773513, the location of gage 14165000. HBVparameterInfo.xlsx, IDU_McKenzie.dbf, Reach_McKenzie.dbf, McKenzieSummary.xlsx - Add Smith47, SFork48, and Lookout49. WaterRights.cpp - Add Smith47, SFork48, and Lookout49. Move the pour point for Mohawk25 from 23773507 to 23773513. Make some cosmetic changes to PopulateHBVCALIB() for legibility and brevity.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55B4787-A448-4318-B85E-2310DFAECDBE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C466D6-7F59-4E24-B4A9-C9380B232EE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="35745" yWindow="-5340" windowWidth="18900" windowHeight="13845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature values" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="HBV" localSheetId="2">'for CSV file'!$A$30:$K$44</definedName>
-    <definedName name="HBV" localSheetId="1">'Table for report'!$B$27:$K$41</definedName>
+    <definedName name="HBV" localSheetId="1">'Table for report'!$C$27:$L$41</definedName>
     <definedName name="HBV_1" localSheetId="1">'Table for report'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="116">
   <si>
     <t>HBV parameter ranges</t>
   </si>
@@ -447,6 +447,33 @@
   </si>
   <si>
     <t>from 9 Blue River Reservoir drainage</t>
+  </si>
+  <si>
+    <t>SMITH RIVER ABV SMITH R RESV NR BELKNAP SPRNGS</t>
+  </si>
+  <si>
+    <t>SO FK MCKENZIE RIVER ABV COUGAR LAKE NR RAINBOW</t>
+  </si>
+  <si>
+    <t>LOOKOUT CREEK NEAR BLUE RIVER</t>
+  </si>
+  <si>
+    <t>ClearLake46</t>
+  </si>
+  <si>
+    <t>Smith47</t>
+  </si>
+  <si>
+    <t>SFork48</t>
+  </si>
+  <si>
+    <t>Lookout49</t>
+  </si>
+  <si>
+    <t>BLU9</t>
+  </si>
+  <si>
+    <t>CGR8</t>
   </si>
 </sst>
 </file>
@@ -602,7 +629,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -788,6 +815,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -960,7 +993,7 @@
     <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1136,6 +1169,10 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -2515,84 +2552,82 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:N52"/>
+  <dimension ref="A1:O55"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C45" sqref="C45:L45"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="5.6640625" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="24" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="6.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.109375" style="24"/>
-    <col min="13" max="13" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+    <col min="2" max="2" width="46.5546875" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" style="24" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="6.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="6.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.109375" style="24"/>
+    <col min="14" max="14" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="51" t="s">
+    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="40" t="s">
+      <c r="E1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="35" t="s">
+      <c r="F1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="38" t="s">
+      <c r="I1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="39" t="s">
+      <c r="J1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="K1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="L1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="65" t="s">
+      <c r="M1" s="65" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="B2" s="50"/>
-      <c r="C2" s="52" t="s">
+    <row r="2" spans="1:15" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="C2" s="50"/>
+      <c r="D2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="45" t="s">
+      <c r="E2" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="46" t="s">
+      <c r="F2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="47" t="s">
+      <c r="G2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="H2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="48" t="s">
+      <c r="I2" s="48" t="s">
         <v>15</v>
-      </c>
-      <c r="I2" s="49" t="s">
-        <v>19</v>
       </c>
       <c r="J2" s="49" t="s">
         <v>19</v>
@@ -2600,2095 +2635,2170 @@
       <c r="K2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="66" t="s">
+      <c r="L2" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="M2" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" s="11" t="s">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B3" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="5">
-        <v>0</v>
-      </c>
-      <c r="C3" s="24">
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="24">
         <v>6</v>
       </c>
-      <c r="D3" s="36">
+      <c r="E3" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E3" s="21">
+      <c r="F3" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>4.8280000000000003</v>
       </c>
-      <c r="G3" s="24">
+      <c r="H3" s="24">
         <v>0.2</v>
       </c>
-      <c r="H3" s="24">
+      <c r="I3" s="24">
         <v>30.85</v>
       </c>
-      <c r="I3" s="30">
+      <c r="J3" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J3" s="30">
+      <c r="K3" s="30">
         <v>0.151</v>
       </c>
-      <c r="K3" s="30">
+      <c r="L3" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L3" s="24">
-        <v>1</v>
-      </c>
-      <c r="M3" s="5"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
+      <c r="M3" s="24">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="41">
+      <c r="C4" s="5">
+        <v>1</v>
+      </c>
+      <c r="D4" s="41">
         <v>3.735868</v>
       </c>
-      <c r="D4" s="42">
+      <c r="E4" s="42">
         <v>5.6955899999999997E-4</v>
       </c>
-      <c r="E4" s="43">
+      <c r="F4" s="43">
         <v>150.53030000000001</v>
       </c>
-      <c r="F4" s="41">
+      <c r="G4" s="41">
         <v>1.3763369999999999</v>
       </c>
-      <c r="G4" s="41">
+      <c r="H4" s="41">
         <v>0.1968587</v>
       </c>
-      <c r="H4" s="41">
+      <c r="I4" s="41">
         <v>7.2725160000000004</v>
       </c>
-      <c r="I4" s="44">
+      <c r="J4" s="44">
         <v>0.49463750000000001</v>
       </c>
-      <c r="J4" s="44">
+      <c r="K4" s="44">
         <v>0.1270905</v>
       </c>
-      <c r="K4" s="44">
+      <c r="L4" s="44">
         <v>7.69113E-3</v>
       </c>
-      <c r="L4" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A5" s="11" t="s">
+      <c r="M4" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="5">
+      <c r="C5" s="5">
         <v>4</v>
       </c>
-      <c r="C5" s="41">
+      <c r="D5" s="41">
         <v>3.275990009</v>
       </c>
-      <c r="D5" s="42">
+      <c r="E5" s="42">
         <v>8.0292649999999993E-2</v>
       </c>
-      <c r="E5" s="43">
+      <c r="F5" s="43">
         <v>200.52503970000001</v>
       </c>
-      <c r="F5" s="41">
+      <c r="G5" s="41">
         <v>1.3476115470000001</v>
       </c>
-      <c r="G5" s="41">
+      <c r="H5" s="41">
         <v>0.176873103</v>
       </c>
-      <c r="H5" s="41">
+      <c r="I5" s="41">
         <v>0.95709490799999997</v>
       </c>
-      <c r="I5" s="44">
+      <c r="J5" s="44">
         <v>0.54816478499999999</v>
       </c>
-      <c r="J5" s="44">
+      <c r="K5" s="44">
         <v>0.250585526</v>
       </c>
-      <c r="K5" s="44">
+      <c r="L5" s="44">
         <v>6.2221719999999998E-3</v>
       </c>
-      <c r="L5" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A6" s="11" t="s">
+      <c r="M5" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B6" s="5">
+      <c r="C6" s="5">
         <v>5</v>
       </c>
-      <c r="C6" s="41">
+      <c r="D6" s="41">
         <v>2.7441309999999999</v>
       </c>
-      <c r="D6" s="42">
+      <c r="E6" s="42">
         <v>2.6143218999999999E-2</v>
       </c>
-      <c r="E6" s="43">
+      <c r="F6" s="43">
         <v>279.84789999999998</v>
       </c>
-      <c r="F6" s="41">
+      <c r="G6" s="41">
         <v>1.238121</v>
       </c>
-      <c r="G6" s="41">
+      <c r="H6" s="41">
         <v>0.18713589999999999</v>
       </c>
-      <c r="H6" s="41">
+      <c r="I6" s="41">
         <v>1.1127959999999999</v>
       </c>
-      <c r="I6" s="44">
+      <c r="J6" s="44">
         <v>0.58749960000000001</v>
       </c>
-      <c r="J6" s="44">
+      <c r="K6" s="44">
         <v>0.28632210000000002</v>
       </c>
-      <c r="K6" s="44">
+      <c r="L6" s="44">
         <v>3.2199999999999999E-2</v>
       </c>
-      <c r="L6" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A7" s="11" t="s">
+      <c r="M6" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="B7" s="4">
+      <c r="C7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="41">
+      <c r="D7" s="41">
         <v>2.9828299999999999</v>
       </c>
-      <c r="D7" s="42">
+      <c r="E7" s="42">
         <v>5.3843389999999998E-2</v>
       </c>
-      <c r="E7" s="43">
+      <c r="F7" s="43">
         <v>520.94399999999996</v>
       </c>
-      <c r="F7" s="41">
+      <c r="G7" s="41">
         <v>1.0192300000000001</v>
       </c>
-      <c r="G7" s="41">
+      <c r="H7" s="41">
         <v>0.163961</v>
       </c>
-      <c r="H7" s="41">
+      <c r="I7" s="41">
         <v>8.5032599999999992</v>
       </c>
-      <c r="I7" s="44">
+      <c r="J7" s="44">
         <v>0.21887599999999999</v>
       </c>
-      <c r="J7" s="44">
+      <c r="K7" s="44">
         <v>0.151643</v>
       </c>
-      <c r="K7" s="44">
+      <c r="L7" s="44">
         <v>3.6759500000000001E-2</v>
       </c>
-      <c r="L7" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A8" s="11" t="s">
+      <c r="M7" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="B8" s="5">
+      <c r="C8" s="5">
         <v>7</v>
       </c>
-      <c r="C8" s="41">
+      <c r="D8" s="41">
         <v>4.6672200000000004</v>
       </c>
-      <c r="D8" s="42">
+      <c r="E8" s="42">
         <v>3.42195E-2</v>
       </c>
-      <c r="E8" s="43">
+      <c r="F8" s="43">
         <v>391.65899999999999</v>
       </c>
-      <c r="F8" s="41">
+      <c r="G8" s="41">
         <v>2.4958499999999999</v>
       </c>
-      <c r="G8" s="41">
+      <c r="H8" s="41">
         <v>0.19991999999999999</v>
       </c>
-      <c r="H8" s="41">
+      <c r="I8" s="41">
         <v>2.0880000000000001</v>
       </c>
-      <c r="I8" s="44">
+      <c r="J8" s="44">
         <v>0.59253599999999995</v>
       </c>
-      <c r="J8" s="44">
+      <c r="K8" s="44">
         <v>0.29457100000000003</v>
       </c>
-      <c r="K8" s="44">
+      <c r="L8" s="44">
         <v>5.4587960000000001E-3</v>
       </c>
-      <c r="L8" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A9" s="11" t="s">
+      <c r="M8" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="5">
+      <c r="C9" s="5">
         <v>8</v>
       </c>
-      <c r="C9" s="41">
+      <c r="D9" s="41">
         <v>2.6385100000000001</v>
       </c>
-      <c r="D9" s="42">
+      <c r="E9" s="42">
         <v>1.3664000000000001E-2</v>
       </c>
-      <c r="E9" s="43">
+      <c r="F9" s="43">
         <v>330.13099999999997</v>
       </c>
-      <c r="F9" s="41">
+      <c r="G9" s="41">
         <v>1.1132899999999999</v>
       </c>
-      <c r="G9" s="41">
+      <c r="H9" s="41">
         <v>0.19864000000000001</v>
       </c>
-      <c r="H9" s="41">
+      <c r="I9" s="41">
         <v>9.1283499999999993</v>
       </c>
-      <c r="I9" s="44">
+      <c r="J9" s="44">
         <v>0.56917600000000002</v>
       </c>
-      <c r="J9" s="44">
+      <c r="K9" s="44">
         <v>0.23161799999999999</v>
       </c>
-      <c r="K9" s="44">
+      <c r="L9" s="44">
         <v>3.0675999999999998E-2</v>
       </c>
-      <c r="L9" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A10" s="11" t="s">
+      <c r="M9" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>114</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="5">
+      <c r="C10" s="5">
         <v>9</v>
       </c>
-      <c r="C10" s="41">
+      <c r="D10" s="41">
         <v>2.5299999999999998</v>
       </c>
-      <c r="D10" s="42">
+      <c r="E10" s="42">
         <v>5.4128975000000003E-2</v>
       </c>
-      <c r="E10" s="43">
+      <c r="F10" s="43">
         <v>219.77199999999999</v>
       </c>
-      <c r="F10" s="41">
+      <c r="G10" s="41">
         <v>1.1459999999999999</v>
       </c>
-      <c r="G10" s="41">
+      <c r="H10" s="41">
         <v>0.188</v>
       </c>
-      <c r="H10" s="41">
+      <c r="I10" s="41">
         <v>4.4269999999999996</v>
       </c>
-      <c r="I10" s="44">
+      <c r="J10" s="44">
         <v>0.58499999999999996</v>
       </c>
-      <c r="J10" s="44">
+      <c r="K10" s="44">
         <v>0.26</v>
       </c>
-      <c r="K10" s="44">
+      <c r="L10" s="44">
         <v>0.03</v>
       </c>
-      <c r="L10" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A11" s="11" t="s">
+      <c r="M10" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="5">
+      <c r="C11" s="5">
         <v>10</v>
       </c>
-      <c r="C11" s="41">
+      <c r="D11" s="41">
         <v>4.056</v>
       </c>
-      <c r="D11" s="42">
+      <c r="E11" s="42">
         <v>0.01</v>
       </c>
-      <c r="E11" s="43">
+      <c r="F11" s="43">
         <v>191.49</v>
       </c>
-      <c r="F11" s="41">
+      <c r="G11" s="41">
         <v>2.2440000000000002</v>
       </c>
-      <c r="G11" s="41">
+      <c r="H11" s="41">
         <v>0.191</v>
       </c>
-      <c r="H11" s="41">
+      <c r="I11" s="41">
         <v>1.365</v>
       </c>
-      <c r="I11" s="44">
+      <c r="J11" s="44">
         <v>0.53400000000000003</v>
       </c>
-      <c r="J11" s="44">
+      <c r="K11" s="44">
         <v>0.27900000000000003</v>
       </c>
-      <c r="K11" s="44">
+      <c r="L11" s="44">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="L11" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A12" s="11" t="s">
+      <c r="M11" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B12" s="5">
+      <c r="C12" s="5">
         <v>12</v>
       </c>
-      <c r="C12" s="41">
+      <c r="D12" s="41">
         <v>3.4518599999999999</v>
       </c>
-      <c r="D12" s="42">
+      <c r="E12" s="42">
         <v>8.7600000000000004E-3</v>
       </c>
-      <c r="E12" s="43">
+      <c r="F12" s="43">
         <v>148.23099999999999</v>
       </c>
-      <c r="F12" s="41">
+      <c r="G12" s="41">
         <v>1.1392199999999999</v>
       </c>
-      <c r="G12" s="41">
+      <c r="H12" s="41">
         <v>0.19630800000000001</v>
       </c>
-      <c r="H12" s="41">
+      <c r="I12" s="41">
         <v>8.8877400000000009</v>
       </c>
-      <c r="I12" s="44">
+      <c r="J12" s="44">
         <v>0.59656799999999999</v>
       </c>
-      <c r="J12" s="44">
+      <c r="K12" s="44">
         <v>0.29032000000000002</v>
       </c>
-      <c r="K12" s="44">
+      <c r="L12" s="44">
         <v>6.9300000000000004E-3</v>
       </c>
-      <c r="L12" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="11" t="s">
+      <c r="M12" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="B13" s="50">
+      <c r="C13" s="50">
         <v>13</v>
       </c>
-      <c r="C13" s="41">
+      <c r="D13" s="41">
         <v>4.0126023289999999</v>
       </c>
-      <c r="D13" s="42">
+      <c r="E13" s="42">
         <v>6.9926142999999996E-2</v>
       </c>
-      <c r="E13" s="43">
+      <c r="F13" s="43">
         <v>346.86500000000001</v>
       </c>
-      <c r="F13" s="41">
+      <c r="G13" s="41">
         <v>2.07613</v>
       </c>
-      <c r="G13" s="41">
+      <c r="H13" s="41">
         <v>0.183729</v>
       </c>
-      <c r="H13" s="41">
+      <c r="I13" s="41">
         <v>47.257199999999997</v>
       </c>
-      <c r="I13" s="44">
+      <c r="J13" s="44">
         <v>0.17288799999999999</v>
       </c>
-      <c r="J13" s="44">
+      <c r="K13" s="44">
         <v>0.260546</v>
       </c>
-      <c r="K13" s="44">
+      <c r="L13" s="44">
         <v>4.9399999999999999E-2</v>
       </c>
-      <c r="L13" s="41">
+      <c r="M13" s="41">
         <v>1.3233600000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="67" t="s">
+    <row r="14" spans="1:15" s="74" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B14" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="B14" s="68">
+      <c r="C14" s="68">
         <v>15</v>
       </c>
-      <c r="C14" s="69">
-        <f>C3</f>
+      <c r="D14" s="69">
+        <f>D3</f>
         <v>6</v>
       </c>
-      <c r="D14" s="70">
-        <f t="shared" ref="D14:M14" si="0">D3</f>
+      <c r="E14" s="70">
+        <f t="shared" ref="E14:N14" si="0">E3</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E14" s="71">
+      <c r="F14" s="71">
         <f t="shared" si="0"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F14" s="69">
+      <c r="G14" s="69">
         <f t="shared" si="0"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G14" s="69">
+      <c r="H14" s="69">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="H14" s="69">
+      <c r="I14" s="69">
         <f t="shared" si="0"/>
         <v>30.85</v>
       </c>
-      <c r="I14" s="72">
+      <c r="J14" s="72">
         <f t="shared" si="0"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J14" s="72">
+      <c r="K14" s="72">
         <f t="shared" si="0"/>
         <v>0.151</v>
       </c>
-      <c r="K14" s="72">
+      <c r="L14" s="72">
         <f t="shared" si="0"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L14" s="69">
+      <c r="M14" s="69">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="M14" s="73">
+      <c r="N14" s="73">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="N14" s="67" t="s">
+      <c r="O14" s="67" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="67" t="s">
+    <row r="15" spans="1:15" s="74" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="B15" s="68">
+      <c r="C15" s="68">
         <v>16</v>
       </c>
-      <c r="C15" s="69">
-        <f>C14</f>
+      <c r="D15" s="69">
+        <f>D14</f>
         <v>6</v>
       </c>
-      <c r="D15" s="70">
-        <f t="shared" ref="D15:M15" si="1">D14</f>
+      <c r="E15" s="70">
+        <f t="shared" ref="E15:N15" si="1">E14</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E15" s="71">
+      <c r="F15" s="71">
         <f t="shared" si="1"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F15" s="69">
+      <c r="G15" s="69">
         <f t="shared" si="1"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G15" s="69">
+      <c r="H15" s="69">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="H15" s="69">
+      <c r="I15" s="69">
         <f t="shared" si="1"/>
         <v>30.85</v>
       </c>
-      <c r="I15" s="72">
+      <c r="J15" s="72">
         <f t="shared" si="1"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J15" s="72">
+      <c r="K15" s="72">
         <f t="shared" si="1"/>
         <v>0.151</v>
       </c>
-      <c r="K15" s="72">
+      <c r="L15" s="72">
         <f t="shared" si="1"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L15" s="69">
+      <c r="M15" s="69">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="M15" s="73">
+      <c r="N15" s="73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N15" s="67" t="s">
+      <c r="O15" s="67" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="67" t="s">
+    <row r="16" spans="1:15" s="74" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="B16" s="68">
+      <c r="C16" s="68">
         <v>17</v>
       </c>
-      <c r="C16" s="69">
-        <f>C$14</f>
+      <c r="D16" s="69">
+        <f>D$14</f>
         <v>6</v>
       </c>
-      <c r="D16" s="70">
-        <f t="shared" ref="D16:M17" si="2">D$14</f>
+      <c r="E16" s="70">
+        <f t="shared" ref="E16:N17" si="2">E$14</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E16" s="71">
+      <c r="F16" s="71">
         <f t="shared" si="2"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F16" s="69">
+      <c r="G16" s="69">
         <f t="shared" si="2"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G16" s="69">
+      <c r="H16" s="69">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="H16" s="69">
+      <c r="I16" s="69">
         <f t="shared" si="2"/>
         <v>30.85</v>
       </c>
-      <c r="I16" s="72">
+      <c r="J16" s="72">
         <f t="shared" si="2"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J16" s="72">
+      <c r="K16" s="72">
         <f t="shared" si="2"/>
         <v>0.151</v>
       </c>
-      <c r="K16" s="72">
+      <c r="L16" s="72">
         <f t="shared" si="2"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L16" s="69">
+      <c r="M16" s="69">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M16" s="73">
+      <c r="N16" s="73">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N16" s="67" t="s">
+      <c r="O16" s="67" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="74" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="67" t="s">
+    <row r="17" spans="2:15" s="74" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="B17" s="68">
+      <c r="C17" s="68">
         <v>18</v>
       </c>
-      <c r="C17" s="69">
-        <f>C$14</f>
+      <c r="D17" s="69">
+        <f>D$14</f>
         <v>6</v>
       </c>
-      <c r="D17" s="70">
+      <c r="E17" s="70">
         <f t="shared" si="2"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E17" s="71">
+      <c r="F17" s="71">
         <f t="shared" si="2"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F17" s="69">
+      <c r="G17" s="69">
         <f t="shared" si="2"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G17" s="69">
+      <c r="H17" s="69">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="H17" s="69">
+      <c r="I17" s="69">
         <f t="shared" si="2"/>
         <v>30.85</v>
       </c>
-      <c r="I17" s="72">
+      <c r="J17" s="72">
         <f t="shared" si="2"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J17" s="72">
+      <c r="K17" s="72">
         <f t="shared" si="2"/>
         <v>0.151</v>
       </c>
-      <c r="K17" s="72">
+      <c r="L17" s="72">
         <f t="shared" si="2"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L17" s="69">
+      <c r="M17" s="69">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M17" s="73">
+      <c r="N17" s="73">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="N17" s="67" t="s">
+      <c r="O17" s="67" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="58" t="s">
+    <row r="18" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="B18" s="59">
+      <c r="C18" s="59">
         <v>19</v>
       </c>
-      <c r="C18" s="60">
-        <f>C$3</f>
+      <c r="D18" s="60">
+        <f>D$3</f>
         <v>6</v>
       </c>
-      <c r="D18" s="61">
-        <f t="shared" ref="D18:M25" si="3">D$3</f>
+      <c r="E18" s="61">
+        <f t="shared" ref="E18:N25" si="3">E$3</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E18" s="62">
+      <c r="F18" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F18" s="60">
+      <c r="G18" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G18" s="60">
+      <c r="H18" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="H18" s="60">
+      <c r="I18" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="I18" s="63">
+      <c r="J18" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J18" s="63">
+      <c r="K18" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="K18" s="63">
+      <c r="L18" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L18" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M18" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N18" s="58" t="s">
+      <c r="M18" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N18" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O18" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="58" t="s">
+    <row r="19" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="B19" s="59">
+      <c r="C19" s="59">
         <v>20</v>
       </c>
-      <c r="C19" s="60">
-        <f>C$3</f>
+      <c r="D19" s="60">
+        <f>D$3</f>
         <v>6</v>
       </c>
-      <c r="D19" s="61">
+      <c r="E19" s="61">
         <f t="shared" si="3"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E19" s="62">
+      <c r="F19" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F19" s="60">
+      <c r="G19" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G19" s="60">
+      <c r="H19" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="H19" s="60">
+      <c r="I19" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="I19" s="63">
+      <c r="J19" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J19" s="63">
+      <c r="K19" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="K19" s="63">
+      <c r="L19" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L19" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M19" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="58" t="s">
+      <c r="M19" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N19" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="81" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="75" t="s">
+    <row r="20" spans="2:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="B20" s="76">
+      <c r="C20" s="76">
         <v>21</v>
       </c>
-      <c r="C20" s="77">
-        <f>C29</f>
+      <c r="D20" s="77">
+        <f>D29</f>
         <v>6</v>
       </c>
-      <c r="D20" s="82">
-        <f t="shared" ref="D20:L20" si="4">D29</f>
+      <c r="E20" s="82">
+        <f t="shared" ref="E20:M20" si="4">E29</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E20" s="78">
+      <c r="F20" s="78">
         <f t="shared" si="4"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F20" s="77">
+      <c r="G20" s="77">
         <f t="shared" si="4"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G20" s="77">
+      <c r="H20" s="77">
         <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
-      <c r="H20" s="77">
+      <c r="I20" s="77">
         <f t="shared" si="4"/>
         <v>30.85</v>
       </c>
-      <c r="I20" s="79">
+      <c r="J20" s="79">
         <f t="shared" si="4"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J20" s="79">
+      <c r="K20" s="79">
         <f t="shared" si="4"/>
         <v>0.151</v>
       </c>
-      <c r="K20" s="79">
+      <c r="L20" s="79">
         <f t="shared" si="4"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L20" s="77">
+      <c r="M20" s="77">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="M20" s="80">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N20" s="75" t="s">
+      <c r="N20" s="80">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O20" s="75" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="58" t="s">
+    <row r="21" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="B21" s="59">
+      <c r="C21" s="59">
         <v>22</v>
       </c>
-      <c r="C21" s="60">
-        <f t="shared" ref="C21" si="5">C$3</f>
+      <c r="D21" s="60">
+        <f t="shared" ref="D21" si="5">D$3</f>
         <v>6</v>
       </c>
-      <c r="D21" s="61">
+      <c r="E21" s="61">
         <f t="shared" si="3"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E21" s="62">
+      <c r="F21" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F21" s="60">
+      <c r="G21" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G21" s="60">
+      <c r="H21" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="H21" s="60">
+      <c r="I21" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="I21" s="63">
+      <c r="J21" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J21" s="63">
+      <c r="K21" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="K21" s="63">
+      <c r="L21" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L21" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M21" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N21" s="75" t="s">
+      <c r="M21" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N21" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O21" s="75" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="11" t="s">
+    <row r="22" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="B22" s="50">
+      <c r="C22" s="50">
         <v>23</v>
       </c>
-      <c r="C22" s="41">
+      <c r="D22" s="41">
         <v>6</v>
       </c>
-      <c r="D22" s="42">
+      <c r="E22" s="42">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E22" s="11">
+      <c r="F22" s="11">
         <v>430.4239197</v>
       </c>
-      <c r="F22" s="11">
+      <c r="G22" s="11">
         <v>3.0282392499999999</v>
       </c>
-      <c r="G22" s="11">
+      <c r="H22" s="11">
         <v>0.18449613500000001</v>
       </c>
-      <c r="H22" s="41">
+      <c r="I22" s="41">
         <v>27.054830549999998</v>
       </c>
-      <c r="I22" s="44">
+      <c r="J22" s="44">
         <v>0.187399387</v>
       </c>
-      <c r="J22" s="44">
+      <c r="K22" s="44">
         <v>0.199641019</v>
       </c>
-      <c r="K22" s="44">
+      <c r="L22" s="44">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L22" s="41">
+      <c r="M22" s="41">
         <v>1.93418479</v>
       </c>
-      <c r="M22" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="58" t="s">
+      <c r="N22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="59">
+      <c r="C23" s="59">
         <v>24</v>
       </c>
-      <c r="C23" s="60">
-        <f>C$3</f>
+      <c r="D23" s="60">
+        <f>D$3</f>
         <v>6</v>
       </c>
-      <c r="D23" s="61">
+      <c r="E23" s="61">
         <f t="shared" si="3"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E23" s="62">
+      <c r="F23" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F23" s="60">
+      <c r="G23" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G23" s="60">
+      <c r="H23" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="H23" s="60">
+      <c r="I23" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="I23" s="63">
+      <c r="J23" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J23" s="63">
+      <c r="K23" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="K23" s="63">
+      <c r="L23" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L23" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M23" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N23" s="75" t="s">
+      <c r="M23" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N23" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O23" s="75" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="58" t="s">
+    <row r="24" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="B24" s="59">
+      <c r="C24" s="59">
         <v>25</v>
       </c>
-      <c r="C24" s="60">
-        <f>C14</f>
+      <c r="D24" s="60">
+        <f>D14</f>
         <v>6</v>
       </c>
-      <c r="D24" s="61">
-        <f t="shared" ref="D24:L24" si="6">D14</f>
+      <c r="E24" s="61">
+        <f t="shared" ref="E24:M24" si="6">E14</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E24" s="62">
+      <c r="F24" s="62">
         <f t="shared" si="6"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F24" s="60">
+      <c r="G24" s="60">
         <f t="shared" si="6"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G24" s="60">
+      <c r="H24" s="60">
         <f t="shared" si="6"/>
         <v>0.2</v>
       </c>
-      <c r="H24" s="60">
+      <c r="I24" s="60">
         <f t="shared" si="6"/>
         <v>30.85</v>
       </c>
-      <c r="I24" s="63">
+      <c r="J24" s="63">
         <f t="shared" si="6"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J24" s="63">
+      <c r="K24" s="63">
         <f t="shared" si="6"/>
         <v>0.151</v>
       </c>
-      <c r="K24" s="63">
+      <c r="L24" s="63">
         <f t="shared" si="6"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L24" s="60">
+      <c r="M24" s="60">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="M24" s="64">
-        <f t="shared" ref="M24" si="7">M$34</f>
-        <v>0</v>
-      </c>
-      <c r="N24" s="58" t="s">
+      <c r="N24" s="64">
+        <f t="shared" ref="N24" si="7">N$34</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="11" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="58" t="s">
+    <row r="25" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="B25" s="59">
+      <c r="C25" s="59">
         <v>26</v>
       </c>
-      <c r="C25" s="60">
-        <f>C$3</f>
+      <c r="D25" s="60">
+        <f>D$3</f>
         <v>6</v>
       </c>
-      <c r="D25" s="61">
+      <c r="E25" s="61">
         <f t="shared" si="3"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E25" s="62">
+      <c r="F25" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F25" s="60">
+      <c r="G25" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G25" s="60">
+      <c r="H25" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="H25" s="60">
+      <c r="I25" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="I25" s="63">
+      <c r="J25" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J25" s="63">
+      <c r="K25" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="K25" s="63">
+      <c r="L25" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L25" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="M25" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N25" s="58" t="s">
+      <c r="M25" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="N25" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="O25" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A26" s="11" t="s">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="B26" s="5">
+      <c r="C26" s="5">
         <v>27</v>
       </c>
-      <c r="C26" s="24">
+      <c r="D26" s="24">
         <v>6</v>
       </c>
-      <c r="D26" s="36">
+      <c r="E26" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E26" s="21">
+      <c r="F26" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>4.8280000000000003</v>
       </c>
-      <c r="G26" s="24">
+      <c r="H26" s="24">
         <v>0.2</v>
       </c>
-      <c r="H26" s="24">
+      <c r="I26" s="24">
         <v>30.85</v>
       </c>
-      <c r="I26" s="30">
+      <c r="J26" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J26" s="30">
+      <c r="K26" s="30">
         <v>0.151</v>
       </c>
-      <c r="K26" s="30">
+      <c r="L26" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L26" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="11" t="s">
+      <c r="M26" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="B27" s="5">
+      <c r="C27" s="5">
         <v>28</v>
       </c>
-      <c r="C27" s="41">
+      <c r="D27" s="41">
         <v>2.52278</v>
       </c>
-      <c r="D27" s="42">
+      <c r="E27" s="42">
         <v>1.4416E-2</v>
       </c>
-      <c r="E27" s="43">
+      <c r="F27" s="43">
         <v>216.00700000000001</v>
       </c>
-      <c r="F27" s="41">
+      <c r="G27" s="41">
         <v>1.2423200000000001</v>
       </c>
-      <c r="G27" s="41">
+      <c r="H27" s="41">
         <v>0.19489799999999999</v>
       </c>
-      <c r="H27" s="41">
+      <c r="I27" s="41">
         <v>8.8562700000000003</v>
       </c>
-      <c r="I27" s="44">
+      <c r="J27" s="44">
         <v>0.59331199999999995</v>
       </c>
-      <c r="J27" s="44">
+      <c r="K27" s="44">
         <v>0.23660999999999999</v>
       </c>
-      <c r="K27" s="44">
+      <c r="L27" s="44">
         <v>2.3149999999999998E-3</v>
       </c>
-      <c r="L27" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" hidden="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="5">
+      <c r="M27" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" hidden="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="5">
         <v>29</v>
       </c>
-      <c r="C28" s="41">
+      <c r="D28" s="41">
         <v>5.9950850000000004</v>
       </c>
-      <c r="D28" s="42">
+      <c r="E28" s="42">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="E28" s="43">
+      <c r="F28" s="43">
         <v>419.92200000000003</v>
       </c>
-      <c r="F28" s="41">
+      <c r="G28" s="41">
         <v>3.4314650000000002</v>
       </c>
-      <c r="G28" s="41">
+      <c r="H28" s="41">
         <v>0.49019000000000001</v>
       </c>
-      <c r="H28" s="41">
+      <c r="I28" s="41">
         <v>48.445349999999998</v>
       </c>
-      <c r="I28" s="44">
+      <c r="J28" s="44">
         <v>0.28832000000000002</v>
       </c>
-      <c r="J28" s="44">
+      <c r="K28" s="44">
         <v>0.25643850000000001</v>
       </c>
-      <c r="K28" s="44">
+      <c r="L28" s="44">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="L28" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A29" s="11" t="s">
+      <c r="M28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="5">
+      <c r="C29" s="5">
         <v>29</v>
       </c>
-      <c r="C29" s="24">
+      <c r="D29" s="24">
         <v>6</v>
       </c>
-      <c r="D29" s="36">
+      <c r="E29" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E29" s="21">
+      <c r="F29" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>4.8280000000000003</v>
       </c>
-      <c r="G29" s="24">
+      <c r="H29" s="24">
         <v>0.2</v>
       </c>
-      <c r="H29" s="24">
+      <c r="I29" s="24">
         <v>30.85</v>
       </c>
-      <c r="I29" s="30">
+      <c r="J29" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J29" s="30">
+      <c r="K29" s="30">
         <v>0.151</v>
       </c>
-      <c r="K29" s="30">
+      <c r="L29" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L29" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A30" s="11" t="s">
+      <c r="M29" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B30" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="B30" s="5">
+      <c r="C30" s="5">
         <v>30</v>
       </c>
-      <c r="C30" s="60">
-        <f>C$3</f>
+      <c r="D30" s="60">
+        <f>D$3</f>
         <v>6</v>
       </c>
-      <c r="D30" s="61">
-        <f t="shared" ref="D30:M32" si="8">D$3</f>
+      <c r="E30" s="61">
+        <f t="shared" ref="E30:N32" si="8">E$3</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E30" s="62">
+      <c r="F30" s="62">
         <f t="shared" si="8"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F30" s="60">
+      <c r="G30" s="60">
         <f t="shared" si="8"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G30" s="60">
+      <c r="H30" s="60">
         <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="H30" s="60">
+      <c r="I30" s="60">
         <f t="shared" si="8"/>
         <v>30.85</v>
       </c>
-      <c r="I30" s="63">
+      <c r="J30" s="63">
         <f t="shared" si="8"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J30" s="63">
+      <c r="K30" s="63">
         <f t="shared" si="8"/>
         <v>0.151</v>
       </c>
-      <c r="K30" s="63">
+      <c r="L30" s="63">
         <f t="shared" si="8"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L30" s="60">
+      <c r="M30" s="60">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M30" s="64">
+      <c r="N30" s="64">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N30" s="58" t="s">
+      <c r="O30" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A31" s="58" t="s">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B31" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="B31" s="5">
+      <c r="C31" s="5">
         <v>31</v>
       </c>
-      <c r="C31" s="60">
-        <f>C$3</f>
+      <c r="D31" s="60">
+        <f>D$3</f>
         <v>6</v>
       </c>
-      <c r="D31" s="61">
+      <c r="E31" s="61">
         <f t="shared" si="8"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E31" s="62">
+      <c r="F31" s="62">
         <f t="shared" si="8"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F31" s="60">
+      <c r="G31" s="60">
         <f t="shared" si="8"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G31" s="60">
+      <c r="H31" s="60">
         <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="H31" s="60">
+      <c r="I31" s="60">
         <f t="shared" si="8"/>
         <v>30.85</v>
       </c>
-      <c r="I31" s="63">
+      <c r="J31" s="63">
         <f t="shared" si="8"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J31" s="63">
+      <c r="K31" s="63">
         <f t="shared" si="8"/>
         <v>0.151</v>
       </c>
-      <c r="K31" s="63">
+      <c r="L31" s="63">
         <f t="shared" si="8"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L31" s="60">
+      <c r="M31" s="60">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M31" s="64">
+      <c r="N31" s="64">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N31" s="58" t="s">
+      <c r="O31" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B32" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="B32" s="5">
+      <c r="C32" s="5">
         <v>32</v>
       </c>
-      <c r="C32" s="60">
-        <f>C$3</f>
+      <c r="D32" s="60">
+        <f>D$3</f>
         <v>6</v>
       </c>
-      <c r="D32" s="61">
+      <c r="E32" s="61">
         <f t="shared" si="8"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E32" s="62">
+      <c r="F32" s="62">
         <f t="shared" si="8"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="F32" s="60">
+      <c r="G32" s="60">
         <f t="shared" si="8"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="G32" s="60">
+      <c r="H32" s="60">
         <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="H32" s="60">
+      <c r="I32" s="60">
         <f t="shared" si="8"/>
         <v>30.85</v>
       </c>
-      <c r="I32" s="63">
+      <c r="J32" s="63">
         <f t="shared" si="8"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="J32" s="63">
+      <c r="K32" s="63">
         <f t="shared" si="8"/>
         <v>0.151</v>
       </c>
-      <c r="K32" s="63">
+      <c r="L32" s="63">
         <f t="shared" si="8"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L32" s="60">
+      <c r="M32" s="60">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="M32" s="64">
+      <c r="N32" s="64">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="N32" s="58" t="s">
+      <c r="O32" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A33" s="11" t="s">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B33" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="B33" s="5">
+      <c r="C33" s="5">
         <v>33</v>
       </c>
-      <c r="C33" s="54">
+      <c r="D33" s="54">
         <v>6</v>
       </c>
-      <c r="D33" s="56">
+      <c r="E33" s="56">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E33" s="57">
+      <c r="F33" s="57">
         <v>536.05999999999995</v>
       </c>
-      <c r="F33" s="54">
+      <c r="G33" s="54">
         <v>4.8280000000000003</v>
       </c>
-      <c r="G33" s="54">
+      <c r="H33" s="54">
         <v>0.2</v>
       </c>
-      <c r="H33" s="54">
+      <c r="I33" s="54">
         <v>30.85</v>
       </c>
-      <c r="I33" s="55">
+      <c r="J33" s="55">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J33" s="55">
+      <c r="K33" s="55">
         <v>0.151</v>
       </c>
-      <c r="K33" s="55">
+      <c r="L33" s="55">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L33" s="24">
-        <v>1</v>
-      </c>
-      <c r="M33" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A34" s="11" t="s">
+      <c r="M33" s="24">
+        <v>1</v>
+      </c>
+      <c r="N33" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B34" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="5">
+      <c r="C34" s="5">
         <v>34</v>
       </c>
-      <c r="C34" s="41">
+      <c r="D34" s="41">
         <v>2.9778201580000001</v>
       </c>
-      <c r="D34" s="42">
+      <c r="E34" s="42">
         <v>4.6919644000000003E-2</v>
       </c>
-      <c r="E34" s="43">
+      <c r="F34" s="43">
         <v>225.4531403</v>
       </c>
-      <c r="F34" s="41">
+      <c r="G34" s="41">
         <v>4.4965953829999998</v>
       </c>
-      <c r="G34" s="41">
+      <c r="H34" s="41">
         <v>0.19683769300000001</v>
       </c>
-      <c r="H34" s="41">
+      <c r="I34" s="41">
         <v>8.1670780179999998</v>
       </c>
-      <c r="I34" s="44">
+      <c r="J34" s="44">
         <v>0.56690686899999998</v>
       </c>
-      <c r="J34" s="44">
+      <c r="K34" s="44">
         <v>8.1609227000000006E-2</v>
       </c>
-      <c r="K34" s="44">
+      <c r="L34" s="44">
         <v>1.0667369999999999E-3</v>
       </c>
-      <c r="L34" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A35" s="11" t="s">
+      <c r="M34" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B35" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="5">
+      <c r="C35" s="5">
         <v>35</v>
       </c>
-      <c r="C35" s="41">
+      <c r="D35" s="41">
         <v>4.6672200000000004</v>
       </c>
-      <c r="D35" s="42">
+      <c r="E35" s="42">
         <v>3.42195E-2</v>
       </c>
-      <c r="E35" s="43">
+      <c r="F35" s="43">
         <v>391.65899999999999</v>
       </c>
-      <c r="F35" s="41">
+      <c r="G35" s="41">
         <v>2.4958499999999999</v>
       </c>
-      <c r="G35" s="41">
+      <c r="H35" s="41">
         <v>0.19991999999999999</v>
       </c>
-      <c r="H35" s="41">
+      <c r="I35" s="41">
         <v>2.0880000000000001</v>
       </c>
-      <c r="I35" s="44">
+      <c r="J35" s="44">
         <v>0.59253599999999995</v>
       </c>
-      <c r="J35" s="44">
+      <c r="K35" s="44">
         <v>0.29457100000000003</v>
       </c>
-      <c r="K35" s="44">
+      <c r="L35" s="44">
         <v>5.4587960000000001E-3</v>
       </c>
-      <c r="L35" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A36" s="11" t="s">
+      <c r="M35" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B36" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="B36" s="5">
+      <c r="C36" s="5">
         <v>36</v>
       </c>
-      <c r="C36" s="24">
+      <c r="D36" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="D36" s="36">
+      <c r="E36" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="E36" s="21">
+      <c r="F36" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="F36" s="24">
+      <c r="G36" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="G36" s="24">
+      <c r="H36" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="H36" s="24">
+      <c r="I36" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="I36" s="30">
+      <c r="J36" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="J36" s="30">
+      <c r="K36" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="K36" s="30">
+      <c r="L36" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="L36" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
+      <c r="M36" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B37" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="5">
+      <c r="C37" s="5">
         <v>37</v>
       </c>
-      <c r="C37" s="24">
+      <c r="D37" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="D37" s="36">
+      <c r="E37" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="E37" s="21">
+      <c r="F37" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="F37" s="24">
+      <c r="G37" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="G37" s="24">
+      <c r="H37" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="H37" s="24">
+      <c r="I37" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="I37" s="30">
+      <c r="J37" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="J37" s="30">
+      <c r="K37" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="K37" s="30">
+      <c r="L37" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="L37" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A38" s="11" t="s">
+      <c r="M37" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B38" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="B38" s="5">
+      <c r="C38" s="5">
         <v>38</v>
       </c>
-      <c r="C38" s="24">
+      <c r="D38" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="D38" s="36">
+      <c r="E38" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="E38" s="21">
+      <c r="F38" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="F38" s="24">
+      <c r="G38" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="G38" s="24">
+      <c r="H38" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="H38" s="24">
+      <c r="I38" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="I38" s="30">
+      <c r="J38" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="J38" s="30">
+      <c r="K38" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="K38" s="30">
+      <c r="L38" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="L38" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A39" s="11" t="s">
+      <c r="M38" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B39" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="B39" s="5">
+      <c r="C39" s="5">
         <v>39</v>
       </c>
-      <c r="C39" s="24">
+      <c r="D39" s="24">
         <v>6</v>
       </c>
-      <c r="D39" s="36">
+      <c r="E39" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E39" s="21">
+      <c r="F39" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>4.8280000000000003</v>
       </c>
-      <c r="G39" s="24">
+      <c r="H39" s="24">
         <v>0.2</v>
       </c>
-      <c r="H39" s="24">
+      <c r="I39" s="24">
         <v>30.85</v>
       </c>
-      <c r="I39" s="30">
+      <c r="J39" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J39" s="30">
+      <c r="K39" s="30">
         <v>0.151</v>
       </c>
-      <c r="K39" s="30">
+      <c r="L39" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L39" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A40" s="11" t="s">
+      <c r="M39" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B40" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="B40" s="5">
+      <c r="C40" s="5">
         <v>41</v>
       </c>
-      <c r="C40" s="24">
+      <c r="D40" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="D40" s="36">
+      <c r="E40" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="E40" s="21">
+      <c r="F40" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="F40" s="24">
+      <c r="G40" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="G40" s="24">
+      <c r="H40" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="H40" s="24">
+      <c r="I40" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="I40" s="30">
+      <c r="J40" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="J40" s="30">
+      <c r="K40" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="K40" s="30">
+      <c r="L40" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="L40" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A41" s="11" t="s">
+      <c r="M40" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B41" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="B41" s="5">
+      <c r="C41" s="5">
         <v>42</v>
       </c>
-      <c r="C41" s="24">
+      <c r="D41" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="D41" s="36">
+      <c r="E41" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="E41" s="21">
+      <c r="F41" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="F41" s="24">
+      <c r="G41" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="G41" s="24">
+      <c r="H41" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="H41" s="24">
+      <c r="I41" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="I41" s="30">
+      <c r="J41" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="J41" s="30">
+      <c r="K41" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="K41" s="30">
+      <c r="L41" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="L41" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A42" s="11" t="s">
+      <c r="M41" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B42" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="B42" s="5">
+      <c r="C42" s="5">
         <v>43</v>
       </c>
-      <c r="C42" s="24">
+      <c r="D42" s="24">
         <v>6</v>
       </c>
-      <c r="D42" s="36">
+      <c r="E42" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E42" s="21">
+      <c r="F42" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="F42">
+      <c r="G42">
         <v>4.8280000000000003</v>
       </c>
-      <c r="G42" s="24">
+      <c r="H42" s="24">
         <v>0.2</v>
       </c>
-      <c r="H42" s="24">
+      <c r="I42" s="24">
         <v>30.85</v>
       </c>
-      <c r="I42" s="30">
+      <c r="J42" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J42" s="30">
+      <c r="K42" s="30">
         <v>0.151</v>
       </c>
-      <c r="K42" s="30">
+      <c r="L42" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L42" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A43" s="11" t="s">
+      <c r="M42" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="B43" s="5">
+      <c r="C43" s="5">
         <v>44</v>
       </c>
-      <c r="C43" s="24">
+      <c r="D43" s="24">
         <v>6</v>
       </c>
-      <c r="D43" s="36">
+      <c r="E43" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E43" s="21">
+      <c r="F43" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="F43">
+      <c r="G43">
         <v>4.8280000000000003</v>
       </c>
-      <c r="G43" s="24">
+      <c r="H43" s="24">
         <v>0.2</v>
       </c>
-      <c r="H43" s="24">
+      <c r="I43" s="24">
         <v>30.85</v>
       </c>
-      <c r="I43" s="30">
+      <c r="J43" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J43" s="30">
+      <c r="K43" s="30">
         <v>0.151</v>
       </c>
-      <c r="K43" s="30">
+      <c r="L43" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L43" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A44" s="11" t="s">
+      <c r="M43" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B44" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="B44" s="5">
+      <c r="C44" s="5">
         <v>45</v>
       </c>
-      <c r="C44" s="24">
+      <c r="D44" s="24">
         <v>6</v>
       </c>
-      <c r="D44" s="36">
+      <c r="E44" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="E44" s="21">
+      <c r="F44" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="F44">
+      <c r="G44">
         <v>4.8280000000000003</v>
       </c>
-      <c r="G44" s="24">
+      <c r="H44" s="24">
         <v>0.2</v>
       </c>
-      <c r="H44" s="24">
+      <c r="I44" s="24">
         <v>30.85</v>
       </c>
-      <c r="I44" s="30">
+      <c r="J44" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="J44" s="30">
+      <c r="K44" s="30">
         <v>0.151</v>
       </c>
-      <c r="K44" s="30">
+      <c r="L44" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="L44" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A45" s="11" t="s">
+      <c r="M44" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>110</v>
+      </c>
+      <c r="B45" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="B45" s="5">
+      <c r="C45" s="5">
         <v>46</v>
       </c>
-      <c r="C45" s="60">
+      <c r="D45" s="60">
         <v>2.5299999999999998</v>
       </c>
-      <c r="D45" s="61">
+      <c r="E45" s="61">
         <v>5.4128975000000003E-2</v>
       </c>
-      <c r="E45" s="62">
+      <c r="F45" s="62">
         <v>219.77199999999999</v>
       </c>
-      <c r="F45" s="60">
+      <c r="G45" s="60">
         <v>1.1459999999999999</v>
       </c>
-      <c r="G45" s="60">
+      <c r="H45" s="60">
         <v>0.188</v>
       </c>
-      <c r="H45" s="60">
+      <c r="I45" s="60">
         <v>4.4269999999999996</v>
       </c>
-      <c r="I45" s="63">
+      <c r="J45" s="63">
         <v>0.58499999999999996</v>
       </c>
-      <c r="J45" s="63">
+      <c r="K45" s="63">
         <v>0.26</v>
       </c>
-      <c r="K45" s="63">
+      <c r="L45" s="63">
         <v>0.03</v>
       </c>
-      <c r="L45" s="60">
-        <v>1</v>
-      </c>
-      <c r="N45" t="s">
+      <c r="M45" s="60">
+        <v>1</v>
+      </c>
+      <c r="O45" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" s="83" t="s">
+        <v>107</v>
+      </c>
+      <c r="C46" s="5">
+        <v>47</v>
+      </c>
+      <c r="D46" s="60"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="62"/>
+      <c r="G46" s="60"/>
+      <c r="H46" s="60"/>
+      <c r="I46" s="60"/>
+      <c r="J46" s="63"/>
+      <c r="K46" s="63"/>
+      <c r="L46" s="63"/>
+      <c r="M46" s="60"/>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>112</v>
+      </c>
+      <c r="B47" s="84" t="s">
+        <v>108</v>
+      </c>
+      <c r="C47" s="5">
+        <v>48</v>
+      </c>
+      <c r="D47" s="60"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="62"/>
+      <c r="G47" s="60"/>
+      <c r="H47" s="60"/>
+      <c r="I47" s="60"/>
+      <c r="J47" s="63"/>
+      <c r="K47" s="63"/>
+      <c r="L47" s="63"/>
+      <c r="M47" s="60"/>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>113</v>
+      </c>
+      <c r="B48" s="84" t="s">
+        <v>109</v>
+      </c>
+      <c r="C48" s="5">
+        <v>49</v>
+      </c>
+      <c r="D48" s="60"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="62"/>
+      <c r="G48" s="60"/>
+      <c r="H48" s="60"/>
+      <c r="I48" s="60"/>
+      <c r="J48" s="63"/>
+      <c r="K48" s="63"/>
+      <c r="L48" s="63"/>
+      <c r="M48" s="60"/>
+    </row>
+    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="24">
+      <c r="C50" s="9"/>
+      <c r="D50" s="24">
         <v>2.3140000000000001</v>
       </c>
-      <c r="D47" s="36">
+      <c r="E50" s="36">
         <v>0.05</v>
       </c>
-      <c r="E47" s="21">
+      <c r="F50" s="21">
         <v>85</v>
       </c>
-      <c r="F47" s="24">
+      <c r="G50" s="24">
         <v>2.15</v>
       </c>
-      <c r="G47" s="24">
+      <c r="H50" s="24">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="H47" s="9">
+      <c r="I50" s="9">
         <v>7.9</v>
       </c>
-      <c r="I47" s="30">
+      <c r="J50" s="30">
         <v>0.13700000000000001</v>
       </c>
-      <c r="J47" s="30">
+      <c r="K50" s="30">
         <v>0.03</v>
       </c>
-      <c r="K47" s="30">
+      <c r="L50" s="30">
         <v>2E-3</v>
       </c>
-      <c r="M47" s="9"/>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="N50" s="9"/>
+    </row>
+    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
         <v>57</v>
       </c>
-      <c r="C48" s="24">
+      <c r="D51" s="24">
         <v>3.72776</v>
       </c>
-      <c r="D48" s="36">
+      <c r="E51" s="36">
         <v>0.05</v>
       </c>
-      <c r="E48" s="21">
+      <c r="F51" s="21">
         <v>456</v>
       </c>
-      <c r="F48" s="24">
+      <c r="G51" s="24">
         <v>4.24</v>
       </c>
-      <c r="G48" s="24">
+      <c r="H51" s="24">
         <v>0.03</v>
       </c>
-      <c r="H48" s="9">
+      <c r="I51" s="9">
         <v>86.6</v>
       </c>
-      <c r="I48" s="30">
+      <c r="J51" s="30">
         <v>0.48</v>
       </c>
-      <c r="J48" s="30">
+      <c r="K51" s="30">
         <v>0.317</v>
       </c>
-      <c r="K48" s="30">
+      <c r="L51" s="30">
         <v>0.105</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
         <v>48</v>
       </c>
-      <c r="C49" s="24">
+      <c r="D52" s="24">
         <v>4.5944700000000003</v>
       </c>
-      <c r="D49" s="36">
+      <c r="E52" s="36">
         <v>8.4928500000000004E-2</v>
       </c>
-      <c r="E49" s="21">
+      <c r="F52" s="21">
         <v>403.43</v>
       </c>
-      <c r="F49" s="24">
+      <c r="G52" s="24">
         <v>3.6036649999999999</v>
       </c>
-      <c r="G49" s="24">
+      <c r="H52" s="24">
         <v>1.5616099999999999</v>
       </c>
-      <c r="H49" s="9">
+      <c r="I52" s="9">
         <v>45.967799999999997</v>
       </c>
-      <c r="I49" s="30">
+      <c r="J52" s="30">
         <v>0.51648300000000003</v>
       </c>
-      <c r="J49" s="30">
+      <c r="K52" s="30">
         <v>0.13280749999999999</v>
       </c>
-      <c r="K49" s="30">
+      <c r="L52" s="30">
         <v>6.1253000000000002E-2</v>
       </c>
-      <c r="M49" s="5" t="s">
+      <c r="N52" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
+    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
         <v>49</v>
       </c>
-      <c r="C50" s="24">
+      <c r="D53" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="D50" s="36">
+      <c r="E53" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="E50" s="21">
+      <c r="F53" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="F50" s="24">
+      <c r="G53" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="G50" s="24">
+      <c r="H53" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="H50" s="9">
+      <c r="I53" s="9">
         <v>48.445349999999998</v>
       </c>
-      <c r="I50" s="30">
+      <c r="J53" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="J50" s="30">
+      <c r="K53" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="K50" s="30">
+      <c r="L53" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="M50" s="5" t="s">
+      <c r="N53" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
+    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
         <v>50</v>
       </c>
-      <c r="C51" s="24">
+      <c r="D54" s="24">
         <v>2.5</v>
       </c>
-      <c r="D51" s="36">
+      <c r="E54" s="36">
         <v>5.3031000000000002E-2</v>
       </c>
-      <c r="E51" s="21">
+      <c r="F54" s="21">
         <v>302.19299999999998</v>
       </c>
-      <c r="F51" s="24">
+      <c r="G54" s="24">
         <v>3.3146300000000002</v>
       </c>
-      <c r="G51" s="24">
+      <c r="H54" s="24">
         <v>0.40926699999999999</v>
       </c>
-      <c r="H51" s="9">
+      <c r="I54" s="9">
         <v>6.09443</v>
       </c>
-      <c r="I51" s="30">
+      <c r="J54" s="30">
         <v>0.24992800000000001</v>
       </c>
-      <c r="J51" s="30">
+      <c r="K54" s="30">
         <v>0.24191099999999999</v>
       </c>
-      <c r="K51" s="30">
+      <c r="L54" s="30">
         <v>8.1710000000000005E-2</v>
       </c>
-      <c r="M51" s="5" t="s">
+      <c r="N54" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
+    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
         <v>51</v>
       </c>
-      <c r="C52" s="24">
+      <c r="D55" s="24">
         <v>2.5</v>
       </c>
-      <c r="D52" s="36">
+      <c r="E55" s="36">
         <v>2.8663500000000001E-2</v>
       </c>
-      <c r="E52" s="21">
+      <c r="F55" s="21">
         <v>51.938099999999999</v>
       </c>
-      <c r="F52" s="24">
+      <c r="G55" s="24">
         <v>2.2341899999999999</v>
       </c>
-      <c r="G52" s="24">
+      <c r="H55" s="24">
         <v>3.267137</v>
       </c>
-      <c r="H52" s="9">
+      <c r="I55" s="9">
         <v>46.490699999999997</v>
       </c>
-      <c r="I52" s="30">
+      <c r="J55" s="30">
         <v>0.25806499999999999</v>
       </c>
-      <c r="J52" s="30">
+      <c r="K55" s="30">
         <v>7.5115000000000001E-2</v>
       </c>
-      <c r="K52" s="30">
+      <c r="L55" s="30">
         <v>4.5275999999999997E-2</v>
       </c>
-      <c r="M52" s="5" t="s">
+      <c r="N55" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -4702,7 +4812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF0CD360-4B2D-45D8-A256-EB9315888EC1}">
   <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F48" sqref="F48:G48"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
FLOWreports_McKenzie.xml - Replace Q with Q_DISCHARG. Flow.cpp, .h - Replace Q with Q_DISCHARG. Update NSantiam and Marys observations to include 2019 and 2020.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C466D6-7F59-4E24-B4A9-C9380B232EE0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F22D02B-0AF2-4AF7-A2A5-ECA24C6BC65A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35745" yWindow="-5340" windowWidth="18900" windowHeight="13845" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature values" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
   </sheets>
   <definedNames>
     <definedName name="HBV" localSheetId="2">'for CSV file'!$A$30:$K$44</definedName>
-    <definedName name="HBV" localSheetId="1">'Table for report'!$C$27:$L$41</definedName>
+    <definedName name="HBV" localSheetId="1">'Table for report'!$E$27:$N$41</definedName>
     <definedName name="HBV_1" localSheetId="1">'Table for report'!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -126,7 +126,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="120">
   <si>
     <t>HBV parameter ranges</t>
   </si>
@@ -474,6 +474,18 @@
   </si>
   <si>
     <t>CGR8</t>
+  </si>
+  <si>
+    <t>LittleNSantiam50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Little N Santiam near Mehama </t>
+  </si>
+  <si>
+    <t>COMID</t>
+  </si>
+  <si>
+    <t>USGS gage</t>
   </si>
 </sst>
 </file>
@@ -2552,2253 +2564,2401 @@
   <sheetPr codeName="Sheet8">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O55"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.88671875" customWidth="1"/>
-    <col min="2" max="2" width="46.5546875" customWidth="1"/>
-    <col min="3" max="3" width="5.6640625" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" style="24" customWidth="1"/>
-    <col min="5" max="5" width="8.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="6.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="6.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.109375" style="24"/>
-    <col min="14" max="14" width="12.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.21875" customWidth="1"/>
+    <col min="2" max="2" width="49.44140625" customWidth="1"/>
+    <col min="3" max="4" width="9" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="7.5546875" style="24" customWidth="1"/>
+    <col min="7" max="7" width="8.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5546875" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.6640625" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.109375" style="24"/>
+    <col min="16" max="16" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="51" t="s">
+    <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="C1" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="F1" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="40" t="s">
+      <c r="G1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="35" t="s">
+      <c r="H1" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="38" t="s">
+      <c r="K1" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="39" t="s">
+      <c r="L1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="39" t="s">
+      <c r="M1" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="39" t="s">
+      <c r="N1" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="65" t="s">
+      <c r="O1" s="65" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.3">
-      <c r="C2" s="50"/>
-      <c r="D2" s="52" t="s">
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+      <c r="E2" s="50"/>
+      <c r="F2" s="52" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="45" t="s">
+      <c r="G2" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="H2" s="46" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="I2" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="47" t="s">
+      <c r="J2" s="47" t="s">
         <v>19</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="K2" s="48" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="49" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="49" t="s">
-        <v>19</v>
       </c>
       <c r="L2" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="66" t="s">
+      <c r="M2" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="49" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B3" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="24">
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="5">
+        <v>0</v>
+      </c>
+      <c r="F3" s="24">
         <v>6</v>
       </c>
-      <c r="E3" s="36">
+      <c r="G3" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F3" s="21">
+      <c r="H3" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <v>4.8280000000000003</v>
       </c>
-      <c r="H3" s="24">
+      <c r="J3" s="24">
         <v>0.2</v>
       </c>
-      <c r="I3" s="24">
+      <c r="K3" s="24">
         <v>30.85</v>
       </c>
-      <c r="J3" s="30">
+      <c r="L3" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K3" s="30">
+      <c r="M3" s="30">
         <v>0.151</v>
       </c>
-      <c r="L3" s="30">
+      <c r="N3" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M3" s="24">
-        <v>1</v>
-      </c>
-      <c r="N3" s="5"/>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O3" s="24">
+        <v>1</v>
+      </c>
+      <c r="P3" s="5"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C4" s="5">
-        <v>1</v>
-      </c>
-      <c r="D4" s="41">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="41">
         <v>3.735868</v>
       </c>
-      <c r="E4" s="42">
+      <c r="G4" s="42">
         <v>5.6955899999999997E-4</v>
       </c>
-      <c r="F4" s="43">
+      <c r="H4" s="43">
         <v>150.53030000000001</v>
       </c>
-      <c r="G4" s="41">
+      <c r="I4" s="41">
         <v>1.3763369999999999</v>
       </c>
-      <c r="H4" s="41">
+      <c r="J4" s="41">
         <v>0.1968587</v>
       </c>
-      <c r="I4" s="41">
+      <c r="K4" s="41">
         <v>7.2725160000000004</v>
       </c>
-      <c r="J4" s="44">
+      <c r="L4" s="44">
         <v>0.49463750000000001</v>
       </c>
-      <c r="K4" s="44">
+      <c r="M4" s="44">
         <v>0.1270905</v>
       </c>
-      <c r="L4" s="44">
+      <c r="N4" s="44">
         <v>7.69113E-3</v>
       </c>
-      <c r="M4" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O4" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="5">
         <v>4</v>
       </c>
-      <c r="D5" s="41">
+      <c r="F5" s="41">
         <v>3.275990009</v>
       </c>
-      <c r="E5" s="42">
+      <c r="G5" s="42">
         <v>8.0292649999999993E-2</v>
       </c>
-      <c r="F5" s="43">
+      <c r="H5" s="43">
         <v>200.52503970000001</v>
       </c>
-      <c r="G5" s="41">
+      <c r="I5" s="41">
         <v>1.3476115470000001</v>
       </c>
-      <c r="H5" s="41">
+      <c r="J5" s="41">
         <v>0.176873103</v>
       </c>
-      <c r="I5" s="41">
+      <c r="K5" s="41">
         <v>0.95709490799999997</v>
       </c>
-      <c r="J5" s="44">
+      <c r="L5" s="44">
         <v>0.54816478499999999</v>
       </c>
-      <c r="K5" s="44">
+      <c r="M5" s="44">
         <v>0.250585526</v>
       </c>
-      <c r="L5" s="44">
+      <c r="N5" s="44">
         <v>6.2221719999999998E-3</v>
       </c>
-      <c r="M5" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O5" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="5">
         <v>5</v>
       </c>
-      <c r="D6" s="41">
+      <c r="F6" s="41">
         <v>2.7441309999999999</v>
       </c>
-      <c r="E6" s="42">
+      <c r="G6" s="42">
         <v>2.6143218999999999E-2</v>
       </c>
-      <c r="F6" s="43">
+      <c r="H6" s="43">
         <v>279.84789999999998</v>
       </c>
-      <c r="G6" s="41">
+      <c r="I6" s="41">
         <v>1.238121</v>
       </c>
-      <c r="H6" s="41">
+      <c r="J6" s="41">
         <v>0.18713589999999999</v>
       </c>
-      <c r="I6" s="41">
+      <c r="K6" s="41">
         <v>1.1127959999999999</v>
       </c>
-      <c r="J6" s="44">
+      <c r="L6" s="44">
         <v>0.58749960000000001</v>
       </c>
-      <c r="K6" s="44">
+      <c r="M6" s="44">
         <v>0.28632210000000002</v>
       </c>
-      <c r="L6" s="44">
+      <c r="N6" s="44">
         <v>3.2199999999999999E-2</v>
       </c>
-      <c r="M6" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O6" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B7" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="4">
         <v>6</v>
       </c>
-      <c r="D7" s="41">
+      <c r="F7" s="41">
         <v>2.9828299999999999</v>
       </c>
-      <c r="E7" s="42">
+      <c r="G7" s="42">
         <v>5.3843389999999998E-2</v>
       </c>
-      <c r="F7" s="43">
+      <c r="H7" s="43">
         <v>520.94399999999996</v>
       </c>
-      <c r="G7" s="41">
+      <c r="I7" s="41">
         <v>1.0192300000000001</v>
       </c>
-      <c r="H7" s="41">
+      <c r="J7" s="41">
         <v>0.163961</v>
       </c>
-      <c r="I7" s="41">
+      <c r="K7" s="41">
         <v>8.5032599999999992</v>
       </c>
-      <c r="J7" s="44">
+      <c r="L7" s="44">
         <v>0.21887599999999999</v>
       </c>
-      <c r="K7" s="44">
+      <c r="M7" s="44">
         <v>0.151643</v>
       </c>
-      <c r="L7" s="44">
+      <c r="N7" s="44">
         <v>3.6759500000000001E-2</v>
       </c>
-      <c r="M7" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O7" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B8" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="5">
         <v>7</v>
       </c>
-      <c r="D8" s="41">
+      <c r="F8" s="41">
         <v>4.6672200000000004</v>
       </c>
-      <c r="E8" s="42">
+      <c r="G8" s="42">
         <v>3.42195E-2</v>
       </c>
-      <c r="F8" s="43">
+      <c r="H8" s="43">
         <v>391.65899999999999</v>
       </c>
-      <c r="G8" s="41">
+      <c r="I8" s="41">
         <v>2.4958499999999999</v>
       </c>
-      <c r="H8" s="41">
+      <c r="J8" s="41">
         <v>0.19991999999999999</v>
       </c>
-      <c r="I8" s="41">
+      <c r="K8" s="41">
         <v>2.0880000000000001</v>
       </c>
-      <c r="J8" s="44">
+      <c r="L8" s="44">
         <v>0.59253599999999995</v>
       </c>
-      <c r="K8" s="44">
+      <c r="M8" s="44">
         <v>0.29457100000000003</v>
       </c>
-      <c r="L8" s="44">
+      <c r="N8" s="44">
         <v>5.4587960000000001E-3</v>
       </c>
-      <c r="M8" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O8" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>115</v>
       </c>
       <c r="B9" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="5">
         <v>8</v>
       </c>
-      <c r="D9" s="41">
+      <c r="F9" s="41">
         <v>2.6385100000000001</v>
       </c>
-      <c r="E9" s="42">
+      <c r="G9" s="42">
         <v>1.3664000000000001E-2</v>
       </c>
-      <c r="F9" s="43">
+      <c r="H9" s="43">
         <v>330.13099999999997</v>
       </c>
-      <c r="G9" s="41">
+      <c r="I9" s="41">
         <v>1.1132899999999999</v>
       </c>
-      <c r="H9" s="41">
+      <c r="J9" s="41">
         <v>0.19864000000000001</v>
       </c>
-      <c r="I9" s="41">
+      <c r="K9" s="41">
         <v>9.1283499999999993</v>
       </c>
-      <c r="J9" s="44">
+      <c r="L9" s="44">
         <v>0.56917600000000002</v>
       </c>
-      <c r="K9" s="44">
+      <c r="M9" s="44">
         <v>0.23161799999999999</v>
       </c>
-      <c r="L9" s="44">
+      <c r="N9" s="44">
         <v>3.0675999999999998E-2</v>
       </c>
-      <c r="M9" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O9" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>114</v>
       </c>
       <c r="B10" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="5">
         <v>9</v>
       </c>
-      <c r="D10" s="41">
+      <c r="F10" s="41">
         <v>2.5299999999999998</v>
       </c>
-      <c r="E10" s="42">
+      <c r="G10" s="42">
         <v>5.4128975000000003E-2</v>
       </c>
-      <c r="F10" s="43">
+      <c r="H10" s="43">
         <v>219.77199999999999</v>
       </c>
-      <c r="G10" s="41">
+      <c r="I10" s="41">
         <v>1.1459999999999999</v>
       </c>
-      <c r="H10" s="41">
+      <c r="J10" s="41">
         <v>0.188</v>
       </c>
-      <c r="I10" s="41">
+      <c r="K10" s="41">
         <v>4.4269999999999996</v>
       </c>
-      <c r="J10" s="44">
+      <c r="L10" s="44">
         <v>0.58499999999999996</v>
       </c>
-      <c r="K10" s="44">
+      <c r="M10" s="44">
         <v>0.26</v>
       </c>
-      <c r="L10" s="44">
+      <c r="N10" s="44">
         <v>0.03</v>
       </c>
-      <c r="M10" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O10" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B11" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="5">
         <v>10</v>
       </c>
-      <c r="D11" s="41">
+      <c r="F11" s="41">
         <v>4.056</v>
       </c>
-      <c r="E11" s="42">
+      <c r="G11" s="42">
         <v>0.01</v>
       </c>
-      <c r="F11" s="43">
+      <c r="H11" s="43">
         <v>191.49</v>
       </c>
-      <c r="G11" s="41">
+      <c r="I11" s="41">
         <v>2.2440000000000002</v>
       </c>
-      <c r="H11" s="41">
+      <c r="J11" s="41">
         <v>0.191</v>
       </c>
-      <c r="I11" s="41">
+      <c r="K11" s="41">
         <v>1.365</v>
       </c>
-      <c r="J11" s="44">
+      <c r="L11" s="44">
         <v>0.53400000000000003</v>
       </c>
-      <c r="K11" s="44">
+      <c r="M11" s="44">
         <v>0.27900000000000003</v>
       </c>
-      <c r="L11" s="44">
+      <c r="N11" s="44">
         <v>6.0999999999999999E-2</v>
       </c>
-      <c r="M11" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O11" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="5">
         <v>12</v>
       </c>
-      <c r="D12" s="41">
+      <c r="F12" s="41">
         <v>3.4518599999999999</v>
       </c>
-      <c r="E12" s="42">
+      <c r="G12" s="42">
         <v>8.7600000000000004E-3</v>
       </c>
-      <c r="F12" s="43">
+      <c r="H12" s="43">
         <v>148.23099999999999</v>
       </c>
-      <c r="G12" s="41">
+      <c r="I12" s="41">
         <v>1.1392199999999999</v>
       </c>
-      <c r="H12" s="41">
+      <c r="J12" s="41">
         <v>0.19630800000000001</v>
       </c>
-      <c r="I12" s="41">
+      <c r="K12" s="41">
         <v>8.8877400000000009</v>
       </c>
-      <c r="J12" s="44">
+      <c r="L12" s="44">
         <v>0.59656799999999999</v>
       </c>
-      <c r="K12" s="44">
+      <c r="M12" s="44">
         <v>0.29032000000000002</v>
       </c>
-      <c r="L12" s="44">
+      <c r="N12" s="44">
         <v>6.9300000000000004E-3</v>
       </c>
-      <c r="M12" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="O12" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B13" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C13" s="50">
+      <c r="E13" s="50">
         <v>13</v>
       </c>
-      <c r="D13" s="41">
+      <c r="F13" s="41">
         <v>4.0126023289999999</v>
       </c>
-      <c r="E13" s="42">
+      <c r="G13" s="42">
         <v>6.9926142999999996E-2</v>
       </c>
-      <c r="F13" s="43">
+      <c r="H13" s="43">
         <v>346.86500000000001</v>
       </c>
-      <c r="G13" s="41">
+      <c r="I13" s="41">
         <v>2.07613</v>
       </c>
-      <c r="H13" s="41">
+      <c r="J13" s="41">
         <v>0.183729</v>
       </c>
-      <c r="I13" s="41">
+      <c r="K13" s="41">
         <v>47.257199999999997</v>
       </c>
-      <c r="J13" s="44">
+      <c r="L13" s="44">
         <v>0.17288799999999999</v>
       </c>
-      <c r="K13" s="44">
+      <c r="M13" s="44">
         <v>0.260546</v>
       </c>
-      <c r="L13" s="44">
+      <c r="N13" s="44">
         <v>4.9399999999999999E-2</v>
       </c>
-      <c r="M13" s="41">
+      <c r="O13" s="41">
         <v>1.3233600000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:15" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B14" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="C14" s="68">
+      <c r="C14" s="67"/>
+      <c r="D14" s="67"/>
+      <c r="E14" s="68">
         <v>15</v>
       </c>
-      <c r="D14" s="69">
-        <f>D3</f>
+      <c r="F14" s="69">
+        <f>F3</f>
         <v>6</v>
       </c>
-      <c r="E14" s="70">
-        <f t="shared" ref="E14:N14" si="0">E3</f>
+      <c r="G14" s="70">
+        <f t="shared" ref="G14:P14" si="0">G3</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F14" s="71">
+      <c r="H14" s="71">
         <f t="shared" si="0"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G14" s="69">
+      <c r="I14" s="69">
         <f t="shared" si="0"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H14" s="69">
+      <c r="J14" s="69">
         <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
-      <c r="I14" s="69">
+      <c r="K14" s="69">
         <f t="shared" si="0"/>
         <v>30.85</v>
       </c>
-      <c r="J14" s="72">
+      <c r="L14" s="72">
         <f t="shared" si="0"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K14" s="72">
+      <c r="M14" s="72">
         <f t="shared" si="0"/>
         <v>0.151</v>
       </c>
-      <c r="L14" s="72">
+      <c r="N14" s="72">
         <f t="shared" si="0"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M14" s="69">
+      <c r="O14" s="69">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="N14" s="73">
+      <c r="P14" s="73">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="O14" s="67" t="s">
+      <c r="Q14" s="67" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B15" s="67" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="68">
+      <c r="C15" s="67"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="68">
         <v>16</v>
       </c>
-      <c r="D15" s="69">
-        <f>D14</f>
+      <c r="F15" s="69">
+        <f>F14</f>
         <v>6</v>
       </c>
-      <c r="E15" s="70">
-        <f t="shared" ref="E15:N15" si="1">E14</f>
+      <c r="G15" s="70">
+        <f t="shared" ref="G15:P15" si="1">G14</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F15" s="71">
+      <c r="H15" s="71">
         <f t="shared" si="1"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G15" s="69">
+      <c r="I15" s="69">
         <f t="shared" si="1"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H15" s="69">
+      <c r="J15" s="69">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="I15" s="69">
+      <c r="K15" s="69">
         <f t="shared" si="1"/>
         <v>30.85</v>
       </c>
-      <c r="J15" s="72">
+      <c r="L15" s="72">
         <f t="shared" si="1"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K15" s="72">
+      <c r="M15" s="72">
         <f t="shared" si="1"/>
         <v>0.151</v>
       </c>
-      <c r="L15" s="72">
+      <c r="N15" s="72">
         <f t="shared" si="1"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M15" s="69">
+      <c r="O15" s="69">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="N15" s="73">
+      <c r="P15" s="73">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O15" s="67" t="s">
+      <c r="Q15" s="67" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:15" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B16" s="67" t="s">
         <v>89</v>
       </c>
-      <c r="C16" s="68">
+      <c r="C16" s="67"/>
+      <c r="D16" s="67"/>
+      <c r="E16" s="68">
         <v>17</v>
       </c>
-      <c r="D16" s="69">
-        <f>D$14</f>
+      <c r="F16" s="69">
+        <f>F$14</f>
         <v>6</v>
       </c>
-      <c r="E16" s="70">
-        <f t="shared" ref="E16:N17" si="2">E$14</f>
+      <c r="G16" s="70">
+        <f t="shared" ref="G16:P17" si="2">G$14</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F16" s="71">
+      <c r="H16" s="71">
         <f t="shared" si="2"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G16" s="69">
+      <c r="I16" s="69">
         <f t="shared" si="2"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H16" s="69">
+      <c r="J16" s="69">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="I16" s="69">
+      <c r="K16" s="69">
         <f t="shared" si="2"/>
         <v>30.85</v>
       </c>
-      <c r="J16" s="72">
+      <c r="L16" s="72">
         <f t="shared" si="2"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K16" s="72">
+      <c r="M16" s="72">
         <f t="shared" si="2"/>
         <v>0.151</v>
       </c>
-      <c r="L16" s="72">
+      <c r="N16" s="72">
         <f t="shared" si="2"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M16" s="69">
+      <c r="O16" s="69">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N16" s="73">
+      <c r="P16" s="73">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O16" s="67" t="s">
+      <c r="Q16" s="67" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="2:15" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B17" s="67" t="s">
         <v>90</v>
       </c>
-      <c r="C17" s="68">
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="68">
         <v>18</v>
       </c>
-      <c r="D17" s="69">
-        <f>D$14</f>
+      <c r="F17" s="69">
+        <f>F$14</f>
         <v>6</v>
       </c>
-      <c r="E17" s="70">
+      <c r="G17" s="70">
         <f t="shared" si="2"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F17" s="71">
+      <c r="H17" s="71">
         <f t="shared" si="2"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G17" s="69">
+      <c r="I17" s="69">
         <f t="shared" si="2"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H17" s="69">
+      <c r="J17" s="69">
         <f t="shared" si="2"/>
         <v>0.2</v>
       </c>
-      <c r="I17" s="69">
+      <c r="K17" s="69">
         <f t="shared" si="2"/>
         <v>30.85</v>
       </c>
-      <c r="J17" s="72">
+      <c r="L17" s="72">
         <f t="shared" si="2"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K17" s="72">
+      <c r="M17" s="72">
         <f t="shared" si="2"/>
         <v>0.151</v>
       </c>
-      <c r="L17" s="72">
+      <c r="N17" s="72">
         <f t="shared" si="2"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M17" s="69">
+      <c r="O17" s="69">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N17" s="73">
+      <c r="P17" s="73">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="O17" s="67" t="s">
+      <c r="Q17" s="67" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B18" s="58" t="s">
         <v>91</v>
       </c>
-      <c r="C18" s="59">
+      <c r="C18" s="58"/>
+      <c r="D18" s="58"/>
+      <c r="E18" s="59">
         <v>19</v>
       </c>
-      <c r="D18" s="60">
-        <f>D$3</f>
+      <c r="F18" s="60">
+        <f>F$3</f>
         <v>6</v>
       </c>
-      <c r="E18" s="61">
-        <f t="shared" ref="E18:N25" si="3">E$3</f>
+      <c r="G18" s="61">
+        <f t="shared" ref="G18:P25" si="3">G$3</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F18" s="62">
+      <c r="H18" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G18" s="60">
+      <c r="I18" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H18" s="60">
+      <c r="J18" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="I18" s="60">
+      <c r="K18" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="J18" s="63">
+      <c r="L18" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K18" s="63">
+      <c r="M18" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="L18" s="63">
+      <c r="N18" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M18" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N18" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O18" s="58" t="s">
+      <c r="O18" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P18" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q18" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="19" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B19" s="58" t="s">
         <v>92</v>
       </c>
-      <c r="C19" s="59">
+      <c r="C19" s="58"/>
+      <c r="D19" s="58"/>
+      <c r="E19" s="59">
         <v>20</v>
       </c>
-      <c r="D19" s="60">
-        <f>D$3</f>
+      <c r="F19" s="60">
+        <f>F$3</f>
         <v>6</v>
       </c>
-      <c r="E19" s="61">
+      <c r="G19" s="61">
         <f t="shared" si="3"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F19" s="62">
+      <c r="H19" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G19" s="60">
+      <c r="I19" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H19" s="60">
+      <c r="J19" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="I19" s="60">
+      <c r="K19" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="J19" s="63">
+      <c r="L19" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K19" s="63">
+      <c r="M19" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="L19" s="63">
+      <c r="N19" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M19" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N19" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="58" t="s">
+      <c r="O19" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P19" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="20" spans="2:15" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" s="81" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B20" s="75" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="76">
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="76">
         <v>21</v>
       </c>
-      <c r="D20" s="77">
-        <f>D29</f>
+      <c r="F20" s="77">
+        <f>F29</f>
         <v>6</v>
       </c>
-      <c r="E20" s="82">
-        <f t="shared" ref="E20:M20" si="4">E29</f>
+      <c r="G20" s="82">
+        <f t="shared" ref="G20:O20" si="4">G29</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F20" s="78">
+      <c r="H20" s="78">
         <f t="shared" si="4"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G20" s="77">
+      <c r="I20" s="77">
         <f t="shared" si="4"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H20" s="77">
+      <c r="J20" s="77">
         <f t="shared" si="4"/>
         <v>0.2</v>
       </c>
-      <c r="I20" s="77">
+      <c r="K20" s="77">
         <f t="shared" si="4"/>
         <v>30.85</v>
       </c>
-      <c r="J20" s="79">
+      <c r="L20" s="79">
         <f t="shared" si="4"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K20" s="79">
+      <c r="M20" s="79">
         <f t="shared" si="4"/>
         <v>0.151</v>
       </c>
-      <c r="L20" s="79">
+      <c r="N20" s="79">
         <f t="shared" si="4"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M20" s="77">
+      <c r="O20" s="77">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="N20" s="80">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O20" s="75" t="s">
+      <c r="P20" s="80">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q20" s="75" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B21" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="C21" s="59">
+      <c r="C21" s="58"/>
+      <c r="D21" s="58"/>
+      <c r="E21" s="59">
         <v>22</v>
       </c>
-      <c r="D21" s="60">
-        <f t="shared" ref="D21" si="5">D$3</f>
+      <c r="F21" s="60">
+        <f t="shared" ref="F21" si="5">F$3</f>
         <v>6</v>
       </c>
-      <c r="E21" s="61">
+      <c r="G21" s="61">
         <f t="shared" si="3"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F21" s="62">
+      <c r="H21" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G21" s="60">
+      <c r="I21" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H21" s="60">
+      <c r="J21" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="I21" s="60">
+      <c r="K21" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="J21" s="63">
+      <c r="L21" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K21" s="63">
+      <c r="M21" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="L21" s="63">
+      <c r="N21" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M21" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N21" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O21" s="75" t="s">
+      <c r="O21" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P21" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="75" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B22" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="50">
+      <c r="E22" s="50">
         <v>23</v>
       </c>
-      <c r="D22" s="41">
+      <c r="F22" s="41">
         <v>6</v>
       </c>
-      <c r="E22" s="42">
+      <c r="G22" s="42">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F22" s="11">
+      <c r="H22" s="11">
         <v>430.4239197</v>
       </c>
-      <c r="G22" s="11">
+      <c r="I22" s="11">
         <v>3.0282392499999999</v>
       </c>
-      <c r="H22" s="11">
+      <c r="J22" s="11">
         <v>0.18449613500000001</v>
       </c>
-      <c r="I22" s="41">
+      <c r="K22" s="41">
         <v>27.054830549999998</v>
       </c>
-      <c r="J22" s="44">
+      <c r="L22" s="44">
         <v>0.187399387</v>
       </c>
-      <c r="K22" s="44">
+      <c r="M22" s="44">
         <v>0.199641019</v>
       </c>
-      <c r="L22" s="44">
+      <c r="N22" s="44">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M22" s="41">
+      <c r="O22" s="41">
         <v>1.93418479</v>
       </c>
-      <c r="N22" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="P22" s="11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B23" s="58" t="s">
         <v>95</v>
       </c>
-      <c r="C23" s="59">
+      <c r="C23" s="58"/>
+      <c r="D23" s="58"/>
+      <c r="E23" s="59">
         <v>24</v>
       </c>
-      <c r="D23" s="60">
-        <f>D$3</f>
+      <c r="F23" s="60">
+        <f>F$3</f>
         <v>6</v>
       </c>
-      <c r="E23" s="61">
+      <c r="G23" s="61">
         <f t="shared" si="3"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F23" s="62">
+      <c r="H23" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G23" s="60">
+      <c r="I23" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H23" s="60">
+      <c r="J23" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="I23" s="60">
+      <c r="K23" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="J23" s="63">
+      <c r="L23" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K23" s="63">
+      <c r="M23" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="L23" s="63">
+      <c r="N23" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M23" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N23" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O23" s="75" t="s">
+      <c r="O23" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P23" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q23" s="75" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B24" s="58" t="s">
         <v>96</v>
       </c>
-      <c r="C24" s="59">
+      <c r="C24" s="58"/>
+      <c r="D24" s="58"/>
+      <c r="E24" s="59">
         <v>25</v>
       </c>
-      <c r="D24" s="60">
-        <f>D14</f>
+      <c r="F24" s="60">
+        <f>F14</f>
         <v>6</v>
       </c>
-      <c r="E24" s="61">
-        <f t="shared" ref="E24:M24" si="6">E14</f>
+      <c r="G24" s="61">
+        <f t="shared" ref="G24:O24" si="6">G14</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F24" s="62">
+      <c r="H24" s="62">
         <f t="shared" si="6"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G24" s="60">
+      <c r="I24" s="60">
         <f t="shared" si="6"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H24" s="60">
+      <c r="J24" s="60">
         <f t="shared" si="6"/>
         <v>0.2</v>
       </c>
-      <c r="I24" s="60">
+      <c r="K24" s="60">
         <f t="shared" si="6"/>
         <v>30.85</v>
       </c>
-      <c r="J24" s="63">
+      <c r="L24" s="63">
         <f t="shared" si="6"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K24" s="63">
+      <c r="M24" s="63">
         <f t="shared" si="6"/>
         <v>0.151</v>
       </c>
-      <c r="L24" s="63">
+      <c r="N24" s="63">
         <f t="shared" si="6"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M24" s="60">
+      <c r="O24" s="60">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="N24" s="64">
-        <f t="shared" ref="N24" si="7">N$34</f>
-        <v>0</v>
-      </c>
-      <c r="O24" s="58" t="s">
+      <c r="P24" s="64">
+        <f t="shared" ref="P24" si="7">P$34</f>
+        <v>0</v>
+      </c>
+      <c r="Q24" s="58" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="25" spans="2:15" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B25" s="58" t="s">
         <v>97</v>
       </c>
-      <c r="C25" s="59">
+      <c r="C25" s="58"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="59">
         <v>26</v>
       </c>
-      <c r="D25" s="60">
-        <f>D$3</f>
+      <c r="F25" s="60">
+        <f>F$3</f>
         <v>6</v>
       </c>
-      <c r="E25" s="61">
+      <c r="G25" s="61">
         <f t="shared" si="3"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F25" s="62">
+      <c r="H25" s="62">
         <f t="shared" si="3"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G25" s="60">
+      <c r="I25" s="60">
         <f t="shared" si="3"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H25" s="60">
+      <c r="J25" s="60">
         <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
-      <c r="I25" s="60">
+      <c r="K25" s="60">
         <f t="shared" si="3"/>
         <v>30.85</v>
       </c>
-      <c r="J25" s="63">
+      <c r="L25" s="63">
         <f t="shared" si="3"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K25" s="63">
+      <c r="M25" s="63">
         <f t="shared" si="3"/>
         <v>0.151</v>
       </c>
-      <c r="L25" s="63">
+      <c r="N25" s="63">
         <f t="shared" si="3"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M25" s="60">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="N25" s="64">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="O25" s="58" t="s">
+      <c r="O25" s="60">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="P25" s="64">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="Q25" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
+      <c r="E26" s="5">
         <v>27</v>
       </c>
-      <c r="D26" s="24">
+      <c r="F26" s="24">
         <v>6</v>
       </c>
-      <c r="E26" s="36">
+      <c r="G26" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F26" s="21">
+      <c r="H26" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="G26">
+      <c r="I26">
         <v>4.8280000000000003</v>
       </c>
-      <c r="H26" s="24">
+      <c r="J26" s="24">
         <v>0.2</v>
       </c>
-      <c r="I26" s="24">
+      <c r="K26" s="24">
         <v>30.85</v>
       </c>
-      <c r="J26" s="30">
+      <c r="L26" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K26" s="30">
+      <c r="M26" s="30">
         <v>0.151</v>
       </c>
-      <c r="L26" s="30">
+      <c r="N26" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M26" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="O26" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="C27" s="5">
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="5">
         <v>28</v>
       </c>
-      <c r="D27" s="41">
+      <c r="F27" s="41">
         <v>2.52278</v>
       </c>
-      <c r="E27" s="42">
+      <c r="G27" s="42">
         <v>1.4416E-2</v>
       </c>
-      <c r="F27" s="43">
+      <c r="H27" s="43">
         <v>216.00700000000001</v>
       </c>
-      <c r="G27" s="41">
+      <c r="I27" s="41">
         <v>1.2423200000000001</v>
       </c>
-      <c r="H27" s="41">
+      <c r="J27" s="41">
         <v>0.19489799999999999</v>
       </c>
-      <c r="I27" s="41">
+      <c r="K27" s="41">
         <v>8.8562700000000003</v>
       </c>
-      <c r="J27" s="44">
+      <c r="L27" s="44">
         <v>0.59331199999999995</v>
       </c>
-      <c r="K27" s="44">
+      <c r="M27" s="44">
         <v>0.23660999999999999</v>
       </c>
-      <c r="L27" s="44">
+      <c r="N27" s="44">
         <v>2.3149999999999998E-3</v>
       </c>
-      <c r="M27" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="2:15" hidden="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="5">
+      <c r="O27" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="2:17" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="5">
         <v>29</v>
       </c>
-      <c r="D28" s="41">
+      <c r="F28" s="41">
         <v>5.9950850000000004</v>
       </c>
-      <c r="E28" s="42">
+      <c r="G28" s="42">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="F28" s="43">
+      <c r="H28" s="43">
         <v>419.92200000000003</v>
       </c>
-      <c r="G28" s="41">
+      <c r="I28" s="41">
         <v>3.4314650000000002</v>
       </c>
-      <c r="H28" s="41">
+      <c r="J28" s="41">
         <v>0.49019000000000001</v>
       </c>
-      <c r="I28" s="41">
+      <c r="K28" s="41">
         <v>48.445349999999998</v>
       </c>
-      <c r="J28" s="44">
+      <c r="L28" s="44">
         <v>0.28832000000000002</v>
       </c>
-      <c r="K28" s="44">
+      <c r="M28" s="44">
         <v>0.25643850000000001</v>
       </c>
-      <c r="L28" s="44">
+      <c r="N28" s="44">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="M28" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O28" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="C29" s="5">
+      <c r="C29" s="11"/>
+      <c r="D29" s="11"/>
+      <c r="E29" s="5">
         <v>29</v>
       </c>
-      <c r="D29" s="24">
+      <c r="F29" s="24">
         <v>6</v>
       </c>
-      <c r="E29" s="36">
+      <c r="G29" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F29" s="21">
+      <c r="H29" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="G29">
+      <c r="I29">
         <v>4.8280000000000003</v>
       </c>
-      <c r="H29" s="24">
+      <c r="J29" s="24">
         <v>0.2</v>
       </c>
-      <c r="I29" s="24">
+      <c r="K29" s="24">
         <v>30.85</v>
       </c>
-      <c r="J29" s="30">
+      <c r="L29" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K29" s="30">
+      <c r="M29" s="30">
         <v>0.151</v>
       </c>
-      <c r="L29" s="30">
+      <c r="N29" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M29" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="O29" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="5">
+      <c r="C30" s="11"/>
+      <c r="D30" s="11"/>
+      <c r="E30" s="5">
         <v>30</v>
       </c>
-      <c r="D30" s="60">
-        <f>D$3</f>
+      <c r="F30" s="60">
+        <f>F$3</f>
         <v>6</v>
       </c>
-      <c r="E30" s="61">
-        <f t="shared" ref="E30:N32" si="8">E$3</f>
+      <c r="G30" s="61">
+        <f t="shared" ref="G30:P32" si="8">G$3</f>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F30" s="62">
+      <c r="H30" s="62">
         <f t="shared" si="8"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G30" s="60">
+      <c r="I30" s="60">
         <f t="shared" si="8"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H30" s="60">
+      <c r="J30" s="60">
         <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="I30" s="60">
+      <c r="K30" s="60">
         <f t="shared" si="8"/>
         <v>30.85</v>
       </c>
-      <c r="J30" s="63">
+      <c r="L30" s="63">
         <f t="shared" si="8"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K30" s="63">
+      <c r="M30" s="63">
         <f t="shared" si="8"/>
         <v>0.151</v>
       </c>
-      <c r="L30" s="63">
+      <c r="N30" s="63">
         <f t="shared" si="8"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M30" s="60">
+      <c r="O30" s="60">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="N30" s="64">
+      <c r="P30" s="64">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O30" s="58" t="s">
+      <c r="Q30" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="58" t="s">
         <v>98</v>
       </c>
-      <c r="C31" s="5">
+      <c r="C31" s="58"/>
+      <c r="D31" s="58"/>
+      <c r="E31" s="5">
         <v>31</v>
       </c>
-      <c r="D31" s="60">
-        <f>D$3</f>
+      <c r="F31" s="60">
+        <f>F$3</f>
         <v>6</v>
       </c>
-      <c r="E31" s="61">
+      <c r="G31" s="61">
         <f t="shared" si="8"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F31" s="62">
+      <c r="H31" s="62">
         <f t="shared" si="8"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G31" s="60">
+      <c r="I31" s="60">
         <f t="shared" si="8"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H31" s="60">
+      <c r="J31" s="60">
         <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="I31" s="60">
+      <c r="K31" s="60">
         <f t="shared" si="8"/>
         <v>30.85</v>
       </c>
-      <c r="J31" s="63">
+      <c r="L31" s="63">
         <f t="shared" si="8"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K31" s="63">
+      <c r="M31" s="63">
         <f t="shared" si="8"/>
         <v>0.151</v>
       </c>
-      <c r="L31" s="63">
+      <c r="N31" s="63">
         <f t="shared" si="8"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M31" s="60">
+      <c r="O31" s="60">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="N31" s="64">
+      <c r="P31" s="64">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O31" s="58" t="s">
+      <c r="Q31" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="C32" s="5">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11"/>
+      <c r="E32" s="5">
         <v>32</v>
       </c>
-      <c r="D32" s="60">
-        <f>D$3</f>
+      <c r="F32" s="60">
+        <f>F$3</f>
         <v>6</v>
       </c>
-      <c r="E32" s="61">
+      <c r="G32" s="61">
         <f t="shared" si="8"/>
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F32" s="62">
+      <c r="H32" s="62">
         <f t="shared" si="8"/>
         <v>536.05999999999995</v>
       </c>
-      <c r="G32" s="60">
+      <c r="I32" s="60">
         <f t="shared" si="8"/>
         <v>4.8280000000000003</v>
       </c>
-      <c r="H32" s="60">
+      <c r="J32" s="60">
         <f t="shared" si="8"/>
         <v>0.2</v>
       </c>
-      <c r="I32" s="60">
+      <c r="K32" s="60">
         <f t="shared" si="8"/>
         <v>30.85</v>
       </c>
-      <c r="J32" s="63">
+      <c r="L32" s="63">
         <f t="shared" si="8"/>
         <v>0.27400000000000002</v>
       </c>
-      <c r="K32" s="63">
+      <c r="M32" s="63">
         <f t="shared" si="8"/>
         <v>0.151</v>
       </c>
-      <c r="L32" s="63">
+      <c r="N32" s="63">
         <f t="shared" si="8"/>
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M32" s="60">
+      <c r="O32" s="60">
         <f t="shared" si="8"/>
         <v>1</v>
       </c>
-      <c r="N32" s="64">
+      <c r="P32" s="64">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="O32" s="58" t="s">
+      <c r="Q32" s="58" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B33" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C33" s="5">
+      <c r="C33" s="11"/>
+      <c r="D33" s="11"/>
+      <c r="E33" s="5">
         <v>33</v>
       </c>
-      <c r="D33" s="54">
+      <c r="F33" s="54">
         <v>6</v>
       </c>
-      <c r="E33" s="56">
+      <c r="G33" s="56">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F33" s="57">
+      <c r="H33" s="57">
         <v>536.05999999999995</v>
       </c>
-      <c r="G33" s="54">
+      <c r="I33" s="54">
         <v>4.8280000000000003</v>
       </c>
-      <c r="H33" s="54">
+      <c r="J33" s="54">
         <v>0.2</v>
       </c>
-      <c r="I33" s="54">
+      <c r="K33" s="54">
         <v>30.85</v>
       </c>
-      <c r="J33" s="55">
+      <c r="L33" s="55">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K33" s="55">
+      <c r="M33" s="55">
         <v>0.151</v>
       </c>
-      <c r="L33" s="55">
+      <c r="N33" s="55">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M33" s="24">
-        <v>1</v>
-      </c>
-      <c r="N33" s="53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O33" s="24">
+        <v>1</v>
+      </c>
+      <c r="P33" s="53">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B34" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="C34" s="5">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11"/>
+      <c r="E34" s="5">
         <v>34</v>
       </c>
-      <c r="D34" s="41">
+      <c r="F34" s="41">
         <v>2.9778201580000001</v>
       </c>
-      <c r="E34" s="42">
+      <c r="G34" s="42">
         <v>4.6919644000000003E-2</v>
       </c>
-      <c r="F34" s="43">
+      <c r="H34" s="43">
         <v>225.4531403</v>
       </c>
-      <c r="G34" s="41">
+      <c r="I34" s="41">
         <v>4.4965953829999998</v>
       </c>
-      <c r="H34" s="41">
+      <c r="J34" s="41">
         <v>0.19683769300000001</v>
       </c>
-      <c r="I34" s="41">
+      <c r="K34" s="41">
         <v>8.1670780179999998</v>
       </c>
-      <c r="J34" s="44">
+      <c r="L34" s="44">
         <v>0.56690686899999998</v>
       </c>
-      <c r="K34" s="44">
+      <c r="M34" s="44">
         <v>8.1609227000000006E-2</v>
       </c>
-      <c r="L34" s="44">
+      <c r="N34" s="44">
         <v>1.0667369999999999E-3</v>
       </c>
-      <c r="M34" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O34" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B35" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C35" s="5">
+      <c r="C35" s="11"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="5">
         <v>35</v>
       </c>
-      <c r="D35" s="41">
+      <c r="F35" s="41">
         <v>4.6672200000000004</v>
       </c>
-      <c r="E35" s="42">
+      <c r="G35" s="42">
         <v>3.42195E-2</v>
       </c>
-      <c r="F35" s="43">
+      <c r="H35" s="43">
         <v>391.65899999999999</v>
       </c>
-      <c r="G35" s="41">
+      <c r="I35" s="41">
         <v>2.4958499999999999</v>
       </c>
-      <c r="H35" s="41">
+      <c r="J35" s="41">
         <v>0.19991999999999999</v>
       </c>
-      <c r="I35" s="41">
+      <c r="K35" s="41">
         <v>2.0880000000000001</v>
       </c>
-      <c r="J35" s="44">
+      <c r="L35" s="44">
         <v>0.59253599999999995</v>
       </c>
-      <c r="K35" s="44">
+      <c r="M35" s="44">
         <v>0.29457100000000003</v>
       </c>
-      <c r="L35" s="44">
+      <c r="N35" s="44">
         <v>5.4587960000000001E-3</v>
       </c>
-      <c r="M35" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O35" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B36" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="C36" s="5">
+      <c r="C36" s="11"/>
+      <c r="D36" s="11"/>
+      <c r="E36" s="5">
         <v>36</v>
       </c>
-      <c r="D36" s="24">
+      <c r="F36" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="E36" s="36">
+      <c r="G36" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="F36" s="21">
+      <c r="H36" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="G36" s="24">
+      <c r="I36" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="H36" s="24">
+      <c r="J36" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="I36" s="24">
+      <c r="K36" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="J36" s="30">
+      <c r="L36" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="K36" s="30">
+      <c r="M36" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="L36" s="30">
+      <c r="N36" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="M36" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O36" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B37" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="C37" s="5">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11"/>
+      <c r="E37" s="5">
         <v>37</v>
       </c>
-      <c r="D37" s="24">
+      <c r="F37" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="E37" s="36">
+      <c r="G37" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="F37" s="21">
+      <c r="H37" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="G37" s="24">
+      <c r="I37" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="H37" s="24">
+      <c r="J37" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="I37" s="24">
+      <c r="K37" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="J37" s="30">
+      <c r="L37" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="K37" s="30">
+      <c r="M37" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="L37" s="30">
+      <c r="N37" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="M37" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O37" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B38" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="C38" s="5">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11"/>
+      <c r="E38" s="5">
         <v>38</v>
       </c>
-      <c r="D38" s="24">
+      <c r="F38" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="E38" s="36">
+      <c r="G38" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="F38" s="21">
+      <c r="H38" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="G38" s="24">
+      <c r="I38" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="H38" s="24">
+      <c r="J38" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="I38" s="24">
+      <c r="K38" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="J38" s="30">
+      <c r="L38" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="K38" s="30">
+      <c r="M38" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="L38" s="30">
+      <c r="N38" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="M38" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O38" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B39" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C39" s="5">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11"/>
+      <c r="E39" s="5">
         <v>39</v>
       </c>
-      <c r="D39" s="24">
+      <c r="F39" s="24">
         <v>6</v>
       </c>
-      <c r="E39" s="36">
+      <c r="G39" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F39" s="21">
+      <c r="H39" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="G39">
+      <c r="I39">
         <v>4.8280000000000003</v>
       </c>
-      <c r="H39" s="24">
+      <c r="J39" s="24">
         <v>0.2</v>
       </c>
-      <c r="I39" s="24">
+      <c r="K39" s="24">
         <v>30.85</v>
       </c>
-      <c r="J39" s="30">
+      <c r="L39" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K39" s="30">
+      <c r="M39" s="30">
         <v>0.151</v>
       </c>
-      <c r="L39" s="30">
+      <c r="N39" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M39" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O39" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B40" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C40" s="5">
+      <c r="C40" s="11"/>
+      <c r="D40" s="11"/>
+      <c r="E40" s="5">
         <v>41</v>
       </c>
-      <c r="D40" s="24">
+      <c r="F40" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="E40" s="36">
+      <c r="G40" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="F40" s="21">
+      <c r="H40" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="G40" s="24">
+      <c r="I40" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="H40" s="24">
+      <c r="J40" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="I40" s="24">
+      <c r="K40" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="J40" s="30">
+      <c r="L40" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="K40" s="30">
+      <c r="M40" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="L40" s="30">
+      <c r="N40" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="M40" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O40" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B41" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="5">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="5">
         <v>42</v>
       </c>
-      <c r="D41" s="24">
+      <c r="F41" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="E41" s="36">
+      <c r="G41" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="F41" s="21">
+      <c r="H41" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="G41" s="24">
+      <c r="I41" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="H41" s="24">
+      <c r="J41" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="I41" s="24">
+      <c r="K41" s="24">
         <v>48.445349999999998</v>
       </c>
-      <c r="J41" s="30">
+      <c r="L41" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="K41" s="30">
+      <c r="M41" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="L41" s="30">
+      <c r="N41" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="M41" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O41" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B42" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C42" s="5">
+      <c r="C42" s="11"/>
+      <c r="D42" s="11"/>
+      <c r="E42" s="5">
         <v>43</v>
       </c>
-      <c r="D42" s="24">
+      <c r="F42" s="24">
         <v>6</v>
       </c>
-      <c r="E42" s="36">
+      <c r="G42" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F42" s="21">
+      <c r="H42" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="G42">
+      <c r="I42">
         <v>4.8280000000000003</v>
       </c>
-      <c r="H42" s="24">
+      <c r="J42" s="24">
         <v>0.2</v>
       </c>
-      <c r="I42" s="24">
+      <c r="K42" s="24">
         <v>30.85</v>
       </c>
-      <c r="J42" s="30">
+      <c r="L42" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K42" s="30">
+      <c r="M42" s="30">
         <v>0.151</v>
       </c>
-      <c r="L42" s="30">
+      <c r="N42" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M42" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O42" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B43" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="5">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11"/>
+      <c r="E43" s="5">
         <v>44</v>
       </c>
-      <c r="D43" s="24">
+      <c r="F43" s="24">
         <v>6</v>
       </c>
-      <c r="E43" s="36">
+      <c r="G43" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F43" s="21">
+      <c r="H43" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="G43">
+      <c r="I43">
         <v>4.8280000000000003</v>
       </c>
-      <c r="H43" s="24">
+      <c r="J43" s="24">
         <v>0.2</v>
       </c>
-      <c r="I43" s="24">
+      <c r="K43" s="24">
         <v>30.85</v>
       </c>
-      <c r="J43" s="30">
+      <c r="L43" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K43" s="30">
+      <c r="M43" s="30">
         <v>0.151</v>
       </c>
-      <c r="L43" s="30">
+      <c r="N43" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M43" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O43" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="B44" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C44" s="5">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11"/>
+      <c r="E44" s="5">
         <v>45</v>
       </c>
-      <c r="D44" s="24">
+      <c r="F44" s="24">
         <v>6</v>
       </c>
-      <c r="E44" s="36">
+      <c r="G44" s="36">
         <v>6.8519999999999998E-2</v>
       </c>
-      <c r="F44" s="21">
+      <c r="H44" s="21">
         <v>536.05999999999995</v>
       </c>
-      <c r="G44">
+      <c r="I44">
         <v>4.8280000000000003</v>
       </c>
-      <c r="H44" s="24">
+      <c r="J44" s="24">
         <v>0.2</v>
       </c>
-      <c r="I44" s="24">
+      <c r="K44" s="24">
         <v>30.85</v>
       </c>
-      <c r="J44" s="30">
+      <c r="L44" s="30">
         <v>0.27400000000000002</v>
       </c>
-      <c r="K44" s="30">
+      <c r="M44" s="30">
         <v>0.151</v>
       </c>
-      <c r="L44" s="30">
+      <c r="N44" s="30">
         <v>5.9999999999999995E-4</v>
       </c>
-      <c r="M44" s="24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O44" s="24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>110</v>
       </c>
       <c r="B45" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C45" s="5">
+      <c r="C45" s="11"/>
+      <c r="D45" s="11"/>
+      <c r="E45" s="5">
         <v>46</v>
       </c>
-      <c r="D45" s="60">
+      <c r="F45" s="60">
         <v>2.5299999999999998</v>
       </c>
-      <c r="E45" s="61">
+      <c r="G45" s="61">
         <v>5.4128975000000003E-2</v>
       </c>
-      <c r="F45" s="62">
+      <c r="H45" s="62">
         <v>219.77199999999999</v>
       </c>
-      <c r="G45" s="60">
+      <c r="I45" s="60">
         <v>1.1459999999999999</v>
       </c>
-      <c r="H45" s="60">
+      <c r="J45" s="60">
         <v>0.188</v>
       </c>
-      <c r="I45" s="60">
+      <c r="K45" s="60">
         <v>4.4269999999999996</v>
       </c>
-      <c r="J45" s="63">
+      <c r="L45" s="63">
         <v>0.58499999999999996</v>
       </c>
-      <c r="K45" s="63">
+      <c r="M45" s="63">
         <v>0.26</v>
       </c>
-      <c r="L45" s="63">
+      <c r="N45" s="63">
         <v>0.03</v>
       </c>
-      <c r="M45" s="60">
-        <v>1</v>
-      </c>
-      <c r="O45" t="s">
+      <c r="O45" s="60">
+        <v>1</v>
+      </c>
+      <c r="Q45" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>111</v>
       </c>
       <c r="B46" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="C46" s="5">
+      <c r="C46" s="83"/>
+      <c r="D46" s="83"/>
+      <c r="E46" s="5">
         <v>47</v>
       </c>
-      <c r="D46" s="60"/>
-      <c r="E46" s="61"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="60"/>
-      <c r="H46" s="60"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="61"/>
+      <c r="H46" s="62"/>
       <c r="I46" s="60"/>
-      <c r="J46" s="63"/>
-      <c r="K46" s="63"/>
+      <c r="J46" s="60"/>
+      <c r="K46" s="60"/>
       <c r="L46" s="63"/>
-      <c r="M46" s="60"/>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M46" s="63"/>
+      <c r="N46" s="63"/>
+      <c r="O46" s="60"/>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>112</v>
       </c>
       <c r="B47" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="84"/>
+      <c r="D47" s="84"/>
+      <c r="E47" s="5">
         <v>48</v>
       </c>
-      <c r="D47" s="60"/>
-      <c r="E47" s="61"/>
-      <c r="F47" s="62"/>
-      <c r="G47" s="60"/>
-      <c r="H47" s="60"/>
+      <c r="F47" s="60"/>
+      <c r="G47" s="61"/>
+      <c r="H47" s="62"/>
       <c r="I47" s="60"/>
-      <c r="J47" s="63"/>
-      <c r="K47" s="63"/>
+      <c r="J47" s="60"/>
+      <c r="K47" s="60"/>
       <c r="L47" s="63"/>
-      <c r="M47" s="60"/>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M47" s="63"/>
+      <c r="N47" s="63"/>
+      <c r="O47" s="60"/>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>113</v>
       </c>
       <c r="B48" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="84"/>
+      <c r="D48" s="84"/>
+      <c r="E48" s="5">
         <v>49</v>
       </c>
-      <c r="D48" s="60"/>
-      <c r="E48" s="61"/>
-      <c r="F48" s="62"/>
-      <c r="G48" s="60"/>
-      <c r="H48" s="60"/>
+      <c r="F48" s="60"/>
+      <c r="G48" s="61"/>
+      <c r="H48" s="62"/>
       <c r="I48" s="60"/>
-      <c r="J48" s="63"/>
-      <c r="K48" s="63"/>
+      <c r="J48" s="60"/>
+      <c r="K48" s="60"/>
       <c r="L48" s="63"/>
-      <c r="M48" s="60"/>
-    </row>
-    <row r="50" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B50" t="s">
+      <c r="M48" s="63"/>
+      <c r="N48" s="63"/>
+      <c r="O48" s="60"/>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49" s="84" t="s">
+        <v>117</v>
+      </c>
+      <c r="C49" s="84"/>
+      <c r="D49" s="84"/>
+      <c r="E49" s="5">
+        <v>50</v>
+      </c>
+      <c r="F49" s="60"/>
+      <c r="G49" s="61"/>
+      <c r="H49" s="62"/>
+      <c r="I49" s="60"/>
+      <c r="J49" s="60"/>
+      <c r="K49" s="60"/>
+      <c r="L49" s="63"/>
+      <c r="M49" s="63"/>
+      <c r="N49" s="63"/>
+      <c r="O49" s="60"/>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B50" s="84"/>
+      <c r="C50" s="84"/>
+      <c r="D50" s="84"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="60"/>
+      <c r="G50" s="61"/>
+      <c r="H50" s="62"/>
+      <c r="I50" s="60"/>
+      <c r="J50" s="60"/>
+      <c r="K50" s="60"/>
+      <c r="L50" s="63"/>
+      <c r="M50" s="63"/>
+      <c r="N50" s="63"/>
+      <c r="O50" s="60"/>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B51" s="84"/>
+      <c r="C51" s="84"/>
+      <c r="D51" s="84"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="60"/>
+      <c r="G51" s="61"/>
+      <c r="H51" s="62"/>
+      <c r="I51" s="60"/>
+      <c r="J51" s="60"/>
+      <c r="K51" s="60"/>
+      <c r="L51" s="63"/>
+      <c r="M51" s="63"/>
+      <c r="N51" s="63"/>
+      <c r="O51" s="60"/>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
         <v>56</v>
       </c>
-      <c r="C50" s="9"/>
-      <c r="D50" s="24">
+      <c r="E53" s="9"/>
+      <c r="F53" s="24">
         <v>2.3140000000000001</v>
       </c>
-      <c r="E50" s="36">
+      <c r="G53" s="36">
         <v>0.05</v>
       </c>
-      <c r="F50" s="21">
+      <c r="H53" s="21">
         <v>85</v>
       </c>
-      <c r="G50" s="24">
+      <c r="I53" s="24">
         <v>2.15</v>
       </c>
-      <c r="H50" s="24">
+      <c r="J53" s="24">
         <v>9.4000000000000004E-3</v>
       </c>
-      <c r="I50" s="9">
+      <c r="K53" s="9">
         <v>7.9</v>
       </c>
-      <c r="J50" s="30">
+      <c r="L53" s="30">
         <v>0.13700000000000001</v>
       </c>
-      <c r="K50" s="30">
+      <c r="M53" s="30">
         <v>0.03</v>
       </c>
-      <c r="L50" s="30">
+      <c r="N53" s="30">
         <v>2E-3</v>
       </c>
-      <c r="N50" s="9"/>
-    </row>
-    <row r="51" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B51" t="s">
+      <c r="P53" s="9"/>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
         <v>57</v>
       </c>
-      <c r="D51" s="24">
+      <c r="F54" s="24">
         <v>3.72776</v>
       </c>
-      <c r="E51" s="36">
+      <c r="G54" s="36">
         <v>0.05</v>
       </c>
-      <c r="F51" s="21">
+      <c r="H54" s="21">
         <v>456</v>
       </c>
-      <c r="G51" s="24">
+      <c r="I54" s="24">
         <v>4.24</v>
       </c>
-      <c r="H51" s="24">
+      <c r="J54" s="24">
         <v>0.03</v>
       </c>
-      <c r="I51" s="9">
+      <c r="K54" s="9">
         <v>86.6</v>
       </c>
-      <c r="J51" s="30">
+      <c r="L54" s="30">
         <v>0.48</v>
       </c>
-      <c r="K51" s="30">
+      <c r="M54" s="30">
         <v>0.317</v>
       </c>
-      <c r="L51" s="30">
+      <c r="N54" s="30">
         <v>0.105</v>
       </c>
     </row>
-    <row r="52" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B52" t="s">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
         <v>48</v>
       </c>
-      <c r="D52" s="24">
+      <c r="F55" s="24">
         <v>4.5944700000000003</v>
       </c>
-      <c r="E52" s="36">
+      <c r="G55" s="36">
         <v>8.4928500000000004E-2</v>
       </c>
-      <c r="F52" s="21">
+      <c r="H55" s="21">
         <v>403.43</v>
       </c>
-      <c r="G52" s="24">
+      <c r="I55" s="24">
         <v>3.6036649999999999</v>
       </c>
-      <c r="H52" s="24">
+      <c r="J55" s="24">
         <v>1.5616099999999999</v>
       </c>
-      <c r="I52" s="9">
+      <c r="K55" s="9">
         <v>45.967799999999997</v>
       </c>
-      <c r="J52" s="30">
+      <c r="L55" s="30">
         <v>0.51648300000000003</v>
       </c>
-      <c r="K52" s="30">
+      <c r="M55" s="30">
         <v>0.13280749999999999</v>
       </c>
-      <c r="L52" s="30">
+      <c r="N55" s="30">
         <v>6.1253000000000002E-2</v>
       </c>
-      <c r="N52" s="5" t="s">
+      <c r="P55" s="5" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B53" t="s">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
         <v>49</v>
       </c>
-      <c r="D53" s="24">
+      <c r="F56" s="24">
         <v>5.9950850000000004</v>
       </c>
-      <c r="E53" s="36">
+      <c r="G56" s="36">
         <v>4.4926000000000001E-2</v>
       </c>
-      <c r="F53" s="21">
+      <c r="H56" s="21">
         <v>419.92200000000003</v>
       </c>
-      <c r="G53" s="24">
+      <c r="I56" s="24">
         <v>3.4314650000000002</v>
       </c>
-      <c r="H53" s="24">
+      <c r="J56" s="24">
         <v>0.49019000000000001</v>
       </c>
-      <c r="I53" s="9">
+      <c r="K56" s="9">
         <v>48.445349999999998</v>
       </c>
-      <c r="J53" s="30">
+      <c r="L56" s="30">
         <v>0.28832000000000002</v>
       </c>
-      <c r="K53" s="30">
+      <c r="M56" s="30">
         <v>0.25643850000000001</v>
       </c>
-      <c r="L53" s="30">
+      <c r="N56" s="30">
         <v>3.7562499999999999E-2</v>
       </c>
-      <c r="N53" s="5" t="s">
+      <c r="P56" s="5" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="54" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B54" t="s">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
         <v>50</v>
       </c>
-      <c r="D54" s="24">
+      <c r="F57" s="24">
         <v>2.5</v>
       </c>
-      <c r="E54" s="36">
+      <c r="G57" s="36">
         <v>5.3031000000000002E-2</v>
       </c>
-      <c r="F54" s="21">
+      <c r="H57" s="21">
         <v>302.19299999999998</v>
       </c>
-      <c r="G54" s="24">
+      <c r="I57" s="24">
         <v>3.3146300000000002</v>
       </c>
-      <c r="H54" s="24">
+      <c r="J57" s="24">
         <v>0.40926699999999999</v>
       </c>
-      <c r="I54" s="9">
+      <c r="K57" s="9">
         <v>6.09443</v>
       </c>
-      <c r="J54" s="30">
+      <c r="L57" s="30">
         <v>0.24992800000000001</v>
       </c>
-      <c r="K54" s="30">
+      <c r="M57" s="30">
         <v>0.24191099999999999</v>
       </c>
-      <c r="L54" s="30">
+      <c r="N57" s="30">
         <v>8.1710000000000005E-2</v>
       </c>
-      <c r="N54" s="5" t="s">
+      <c r="P57" s="5" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="55" spans="2:14" x14ac:dyDescent="0.3">
-      <c r="B55" t="s">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="B58" t="s">
         <v>51</v>
       </c>
-      <c r="D55" s="24">
+      <c r="F58" s="24">
         <v>2.5</v>
       </c>
-      <c r="E55" s="36">
+      <c r="G58" s="36">
         <v>2.8663500000000001E-2</v>
       </c>
-      <c r="F55" s="21">
+      <c r="H58" s="21">
         <v>51.938099999999999</v>
       </c>
-      <c r="G55" s="24">
+      <c r="I58" s="24">
         <v>2.2341899999999999</v>
       </c>
-      <c r="H55" s="24">
+      <c r="J58" s="24">
         <v>3.267137</v>
       </c>
-      <c r="I55" s="9">
+      <c r="K58" s="9">
         <v>46.490699999999997</v>
       </c>
-      <c r="J55" s="30">
+      <c r="L58" s="30">
         <v>0.25806499999999999</v>
       </c>
-      <c r="K55" s="30">
+      <c r="M58" s="30">
         <v>7.5115000000000001E-2</v>
       </c>
-      <c r="L55" s="30">
+      <c r="N58" s="30">
         <v>4.5275999999999997E-2</v>
       </c>
-      <c r="N55" s="5" t="s">
+      <c r="P58" s="5" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CW3M_WRB.envx - Add studyAreaName='WRB'. Move shapefiles to DataCW3M/WRB. Rename shapefiles with WRB suffix instead of CW3M suffix. HBVparameterInfo.xlsx and WaterRights.cpp - Add LittleNSantiam50 and Blowout51.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7744432-B57B-4D65-B0D6-C2C1760ECBBB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24026981-87C0-4832-87D9-707431A886F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature values" sheetId="1" r:id="rId1"/>
@@ -2581,7 +2581,7 @@
   </sheetPr>
   <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Commit OSU's letter about CW3M to the repository.
</commit_message>
<xml_diff>
--- a/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
+++ b/DataCW3M/CW3MdigitalHandbook/HBVparameterInfo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24131"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CW3M.git\trunk\DataCW3M\CW3MdigitalHandbook\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24026981-87C0-4832-87D9-707431A886F2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A4131FC-4BD1-4FCF-9D2F-9B9024010B4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-7425" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="literature values" sheetId="1" r:id="rId1"/>
@@ -1597,30 +1597,30 @@
       <selection pane="bottomRight" activeCell="A29" sqref="A29:XFD31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.109375" customWidth="1"/>
-    <col min="2" max="3" width="7.5546875" style="9" customWidth="1"/>
-    <col min="4" max="5" width="9.109375" style="24"/>
-    <col min="6" max="7" width="9.109375" style="25"/>
-    <col min="8" max="9" width="9.109375" style="9"/>
-    <col min="10" max="11" width="9.109375" style="30"/>
-    <col min="12" max="13" width="9.109375" style="21"/>
-    <col min="14" max="19" width="9.109375" style="24"/>
-    <col min="20" max="20" width="18.33203125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="23.140625" customWidth="1"/>
+    <col min="2" max="3" width="7.5703125" style="9" customWidth="1"/>
+    <col min="4" max="5" width="9.140625" style="24"/>
+    <col min="6" max="7" width="9.140625" style="25"/>
+    <col min="8" max="9" width="9.140625" style="9"/>
+    <col min="10" max="11" width="9.140625" style="30"/>
+    <col min="12" max="13" width="9.140625" style="21"/>
+    <col min="14" max="19" width="9.140625" style="24"/>
+    <col min="20" max="20" width="18.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="10" t="s">
         <v>4</v>
       </c>
@@ -1677,7 +1677,7 @@
       </c>
       <c r="T4" s="6"/>
     </row>
-    <row r="5" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>2</v>
       </c>
@@ -1737,7 +1737,7 @@
       </c>
       <c r="U5" s="5"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1843,7 +1843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1899,7 +1899,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:21" s="7" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>23</v>
       </c>
@@ -1949,7 +1949,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>27</v>
       </c>
@@ -2007,7 +2007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="12"/>
       <c r="C11" s="12"/>
       <c r="D11" s="23"/>
@@ -2028,7 +2028,7 @@
       <c r="S11" s="23"/>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>25</v>
       </c>
@@ -2088,7 +2088,7 @@
       </c>
       <c r="T12" s="6"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>1.6E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>27</v>
       </c>
@@ -2193,12 +2193,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -2230,7 +2230,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -2294,7 +2294,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>21</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -2358,7 +2358,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -2390,7 +2390,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2486,12 +2486,12 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
       <c r="K26" s="30" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>41</v>
       </c>
@@ -2585,24 +2585,24 @@
       <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.21875" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" customWidth="1"/>
+    <col min="1" max="1" width="17.28515625" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" customWidth="1"/>
     <col min="3" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="5.6640625" customWidth="1"/>
-    <col min="6" max="6" width="7.5546875" style="24" customWidth="1"/>
-    <col min="7" max="7" width="8.6640625" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="6.109375" style="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="6.6640625" style="30" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.109375" style="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9.109375" style="24"/>
-    <col min="16" max="16" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="5.7109375" customWidth="1"/>
+    <col min="6" max="6" width="7.5703125" style="24" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="36" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="21" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="6.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="6.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9.140625" style="24"/>
+    <col min="16" max="16" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C1" s="5" t="s">
         <v>117</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:17" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" s="5" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="E2" s="50"/>
       <c r="F2" s="52" t="s">
         <v>17</v>
@@ -2679,7 +2679,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B3" s="11" t="s">
         <v>80</v>
       </c>
@@ -2720,7 +2720,7 @@
       </c>
       <c r="P3" s="5"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>59</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>60</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B6" s="11" t="s">
         <v>61</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="11" t="s">
         <v>62</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="11" t="s">
         <v>63</v>
       </c>
@@ -2920,7 +2920,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>114</v>
       </c>
@@ -2963,7 +2963,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>113</v>
       </c>
@@ -3006,7 +3006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="11" t="s">
         <v>66</v>
       </c>
@@ -3046,7 +3046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>121</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B13" s="11" t="s">
         <v>79</v>
       </c>
@@ -3127,7 +3127,7 @@
         <v>1.3233600000000001</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="67" t="s">
         <v>87</v>
       </c>
@@ -3184,7 +3184,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B15" s="67" t="s">
         <v>86</v>
       </c>
@@ -3241,7 +3241,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="16" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B16" s="67" t="s">
         <v>88</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="17" spans="2:17" s="74" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:17" s="74" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="67" t="s">
         <v>89</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B18" s="58" t="s">
         <v>90</v>
       </c>
@@ -3412,7 +3412,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="58" t="s">
         <v>91</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="2:17" s="81" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:17" s="81" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B20" s="75" t="s">
         <v>92</v>
       </c>
@@ -3526,7 +3526,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="21" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="58" t="s">
         <v>93</v>
       </c>
@@ -3583,7 +3583,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="22" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="11" t="s">
         <v>85</v>
       </c>
@@ -3624,7 +3624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="58" t="s">
         <v>94</v>
       </c>
@@ -3681,7 +3681,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="24" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="58" t="s">
         <v>95</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="25" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:17" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="58" t="s">
         <v>96</v>
       </c>
@@ -3795,7 +3795,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B26" s="11" t="s">
         <v>78</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:17" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="11" t="s">
         <v>68</v>
       </c>
@@ -3875,7 +3875,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="2:17" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:17" hidden="1" x14ac:dyDescent="0.25">
       <c r="E28" s="5">
         <v>29</v>
       </c>
@@ -3910,7 +3910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B29" s="11" t="s">
         <v>77</v>
       </c>
@@ -3950,7 +3950,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B30" s="11" t="s">
         <v>101</v>
       </c>
@@ -4007,7 +4007,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B31" s="58" t="s">
         <v>97</v>
       </c>
@@ -4064,7 +4064,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
       <c r="B32" s="11" t="s">
         <v>102</v>
       </c>
@@ -4121,7 +4121,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B33" s="11" t="s">
         <v>84</v>
       </c>
@@ -4164,7 +4164,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B34" s="11" t="s">
         <v>69</v>
       </c>
@@ -4204,7 +4204,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B35" s="11" t="s">
         <v>70</v>
       </c>
@@ -4244,7 +4244,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B36" s="11" t="s">
         <v>71</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>122</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>73</v>
       </c>
@@ -4367,7 +4367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>74</v>
       </c>
@@ -4407,7 +4407,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B40" s="11" t="s">
         <v>75</v>
       </c>
@@ -4447,7 +4447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B41" s="11" t="s">
         <v>76</v>
       </c>
@@ -4487,7 +4487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B42" s="11" t="s">
         <v>81</v>
       </c>
@@ -4527,7 +4527,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>123</v>
       </c>
@@ -4570,7 +4570,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B44" s="11" t="s">
         <v>82</v>
       </c>
@@ -4610,7 +4610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>109</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>110</v>
       </c>
@@ -4679,7 +4679,7 @@
       <c r="N46" s="63"/>
       <c r="O46" s="60"/>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>111</v>
       </c>
@@ -4702,7 +4702,7 @@
       <c r="N47" s="63"/>
       <c r="O47" s="60"/>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>112</v>
       </c>
@@ -4725,7 +4725,7 @@
       <c r="N48" s="63"/>
       <c r="O48" s="60"/>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>115</v>
       </c>
@@ -4748,7 +4748,7 @@
       <c r="N49" s="63"/>
       <c r="O49" s="60"/>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>119</v>
       </c>
@@ -4771,7 +4771,7 @@
       <c r="N50" s="63"/>
       <c r="O50" s="60"/>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B51" s="84"/>
       <c r="C51" s="84"/>
       <c r="D51" s="84"/>
@@ -4787,7 +4787,7 @@
       <c r="N51" s="63"/>
       <c r="O51" s="60"/>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>56</v>
       </c>
@@ -4821,7 +4821,7 @@
       </c>
       <c r="P53" s="9"/>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>57</v>
       </c>
@@ -4853,7 +4853,7 @@
         <v>0.105</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>48</v>
       </c>
@@ -4888,7 +4888,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>49</v>
       </c>
@@ -4923,7 +4923,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
         <v>50</v>
       </c>
@@ -4958,7 +4958,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>51</v>
       </c>
@@ -5007,13 +5007,13 @@
       <selection activeCell="F48" sqref="F48:G48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="9.109375" style="24"/>
-    <col min="6" max="7" width="9.109375" style="36"/>
+    <col min="5" max="5" width="9.140625" style="24"/>
+    <col min="6" max="7" width="9.140625" style="36"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="51" t="s">
         <v>45</v>
       </c>
@@ -5051,7 +5051,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -5089,7 +5089,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -5127,7 +5127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -5165,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -5203,7 +5203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -5241,7 +5241,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -5279,7 +5279,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -5317,7 +5317,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="5">
         <v>7</v>
       </c>
@@ -5355,7 +5355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>8</v>
       </c>
@@ -5393,7 +5393,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="5">
         <v>9</v>
       </c>
@@ -5431,7 +5431,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>11</v>
       </c>
@@ -5507,7 +5507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="5">
         <v>12</v>
       </c>
@@ -5545,7 +5545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="50">
         <v>13</v>
       </c>
@@ -5583,7 +5583,7 @@
         <v>1.3233600000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="59">
         <v>14</v>
       </c>
@@ -5621,7 +5621,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="59">
         <v>15</v>
       </c>
@@ -5669,7 +5669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="59">
         <v>16</v>
       </c>
@@ -5717,7 +5717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="59">
         <v>17</v>
       </c>
@@ -5765,7 +5765,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="59">
         <v>18</v>
       </c>
@@ -5813,7 +5813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="59">
         <v>19</v>
       </c>
@@ -5861,7 +5861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="59">
         <v>20</v>
       </c>
@@ -5909,7 +5909,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="59">
         <v>21</v>
       </c>
@@ -5957,7 +5957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="59">
         <v>22</v>
       </c>
@@ -6005,7 +6005,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="50">
         <v>23</v>
       </c>
@@ -6043,7 +6043,7 @@
         <v>1.93418479</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="59">
         <v>24</v>
       </c>
@@ -6091,7 +6091,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="59">
         <v>25</v>
       </c>
@@ -6139,7 +6139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="59">
         <v>26</v>
       </c>
@@ -6187,7 +6187,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>27</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>28</v>
       </c>
@@ -6263,7 +6263,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>29</v>
       </c>
@@ -6301,7 +6301,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>30</v>
       </c>
@@ -6339,7 +6339,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>31</v>
       </c>
@@ -6387,7 +6387,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="5">
         <v>32</v>
       </c>
@@ -6435,7 +6435,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>33</v>
       </c>
@@ -6473,7 +6473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>34</v>
       </c>
@@ -6511,7 +6511,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="5">
         <v>35</v>
       </c>
@@ -6549,7 +6549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="5">
         <v>36</v>
       </c>
@@ -6587,7 +6587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="5">
         <v>37</v>
       </c>
@@ -6625,7 +6625,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="5">
         <v>38</v>
       </c>
@@ -6663,7 +6663,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="5">
         <v>39</v>
       </c>
@@ -6701,7 +6701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="5">
         <v>40</v>
       </c>
@@ -6739,7 +6739,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="5">
         <v>41</v>
       </c>
@@ -6777,7 +6777,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="5">
         <v>42</v>
       </c>
@@ -6815,7 +6815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="5">
         <v>43</v>
       </c>
@@ -6853,7 +6853,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="5">
         <v>44</v>
       </c>
@@ -6891,7 +6891,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="5">
         <v>45</v>
       </c>
@@ -6929,7 +6929,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="5">
         <v>46</v>
       </c>

</xml_diff>